<commit_message>
Discussion of product and behaviour
</commit_message>
<xml_diff>
--- a/inputs/AddictO_HUman_behaviour_Defs.xlsx
+++ b/inputs/AddictO_HUman_behaviour_Defs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f3488854ec43ae20/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{16CC20F6-0111-43A1-8709-BB826C1517B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D5B214AE-B110-474D-B4F2-B2D35E5F49FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5732E45-81D5-4C3F-86FE-CB90DC2CE02D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="630">
   <si>
     <t>ID</t>
   </si>
@@ -430,9 +430,6 @@
     <t>Abstinence</t>
   </si>
   <si>
-    <t>The behaviour of not performing an action that has previously been habitual.</t>
-  </si>
-  <si>
     <t>Dependent continuant</t>
   </si>
   <si>
@@ -1777,9 +1774,6 @@
     <t>A representation of a behaviour of a person in which that person is believed to have committed suicide.</t>
   </si>
   <si>
-    <t>Product use behaviour in which the product is a psychoactive substance and the purpose is not consistent with legal or medical guidelines.</t>
-  </si>
-  <si>
     <t>Cross reference</t>
   </si>
   <si>
@@ -1849,9 +1843,6 @@
     <t>Proccess (or state?)</t>
   </si>
   <si>
-    <t>A consumption behaviour pattern that involves use of a psychoactive substance by an adolescent that has not been legally sanctioned in the jurisdiction in which the user resides.</t>
-  </si>
-  <si>
     <t>Consumption behaviour pattern, Substance use, adolescent</t>
   </si>
   <si>
@@ -1876,12 +1867,6 @@
     <t>A consumption behaviour that involves drinking an alcohol-containing product.</t>
   </si>
   <si>
-    <t>Pattern of use of a substance containing alcohol by an adolescent.</t>
-  </si>
-  <si>
-    <t>Alcohol use that exhibits the attribute of abstinence.</t>
-  </si>
-  <si>
     <t>A consumption behaviour patterns involving use of a substance containing alcohol concurrently with use of a psychoactice substance that has not been legally sanctioned in the jusridiction in which the user resides.</t>
   </si>
   <si>
@@ -1901,13 +1886,46 @@
   </si>
   <si>
     <t>Consumption of alcohol in a manner that is deemed to cause harm to the individual, others or society.</t>
+  </si>
+  <si>
+    <t>A consumption behaviour that involves ingesting a psychoactive substance.</t>
+  </si>
+  <si>
+    <t>Substance use that is judged to be problematic by a social group.</t>
+  </si>
+  <si>
+    <t>The judgement of misuse is realtive to a social group. This does not mean something is substance misuse if it is judged to be problematic by any social group.</t>
+  </si>
+  <si>
+    <t>'Substance use' and 'has agent' some adolescent</t>
+  </si>
+  <si>
+    <t>Drinking pattern' and 'has agent' some adolescent</t>
+  </si>
+  <si>
+    <t>A drinking pattern by an adolescent.</t>
+  </si>
+  <si>
+    <t>Substance use by an adolescent.</t>
+  </si>
+  <si>
+    <t>A process attribute of alcohol consumption that involves its temporal organisation.</t>
+  </si>
+  <si>
+    <t>Abstinence in alcohol consumption.</t>
+  </si>
+  <si>
+    <t>The behaviour of not performing a behaviour of a particular type.</t>
+  </si>
+  <si>
+    <t>Abstinence only has any meaning when specifying what the behaviour is that the person is not doing.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1978,6 +1996,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1999,7 +2024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2067,6 +2092,21 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2406,8 +2446,8 @@
   <dimension ref="A1:T422"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2445,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>59</v>
@@ -2490,7 +2530,7 @@
         <v>117</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
@@ -2553,7 +2593,7 @@
         <v>128</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>129</v>
@@ -2579,10 +2619,10 @@
         <v>130</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>577</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>578</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>62</v>
@@ -2600,46 +2640,48 @@
       <c r="S5" s="13"/>
       <c r="T5" s="11"/>
     </row>
-    <row r="6" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:20" s="25" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="B6" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="25" t="s">
+        <v>628</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="O6" s="12" t="s">
+      <c r="G6" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="O6" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="Q6" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="S6" s="13"/>
-      <c r="T6" s="11"/>
+      <c r="Q6" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="S6" s="28"/>
+      <c r="T6" s="26"/>
     </row>
     <row r="7" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>263</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
         <v>76</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>4</v>
@@ -2662,10 +2704,10 @@
     </row>
     <row r="8" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>129</v>
@@ -2689,14 +2731,14 @@
     <row r="9" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>61</v>
@@ -2722,13 +2764,13 @@
     </row>
     <row r="10" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>61</v>
@@ -2748,13 +2790,13 @@
     </row>
     <row r="11" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>140</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>77</v>
@@ -2778,16 +2820,16 @@
     <row r="12" spans="1:20" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="16" t="s">
+        <v>606</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>607</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>609</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>610</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>612</v>
-      </c>
       <c r="E12" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>61</v>
@@ -2797,10 +2839,10 @@
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
@@ -2820,14 +2862,16 @@
     <row r="13" spans="1:20" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>606</v>
-      </c>
-      <c r="D13" s="10"/>
+        <v>625</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>622</v>
+      </c>
       <c r="E13" s="10" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>61</v>
@@ -2856,14 +2900,16 @@
     <row r="14" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>615</v>
-      </c>
-      <c r="D14" s="10"/>
+        <v>624</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>623</v>
+      </c>
       <c r="E14" s="10" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>61</v>
@@ -2892,17 +2938,17 @@
     <row r="15" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>616</v>
+        <v>627</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>4</v>
@@ -2925,14 +2971,14 @@
     <row r="16" spans="1:20" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>61</v>
@@ -2958,10 +3004,10 @@
     <row r="17" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="23" t="s">
@@ -2989,10 +3035,10 @@
     <row r="18" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="23" t="s">
@@ -3020,10 +3066,10 @@
     <row r="19" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="23" t="s">
@@ -3051,10 +3097,10 @@
     <row r="20" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="23" t="s">
@@ -3082,10 +3128,10 @@
     <row r="21" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="23" t="s">
@@ -3113,14 +3159,14 @@
     <row r="22" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
@@ -3144,7 +3190,7 @@
     <row r="23" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -3171,10 +3217,10 @@
     <row r="24" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="16"/>
       <c r="B24" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16" t="s">
@@ -3189,7 +3235,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
@@ -3198,7 +3244,7 @@
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
       <c r="Q24" s="16" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
@@ -3206,12 +3252,12 @@
     <row r="25" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
@@ -3235,7 +3281,7 @@
     <row r="26" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -3262,7 +3308,7 @@
     <row r="27" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -3289,10 +3335,10 @@
     <row r="28" spans="1:19" s="12" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>287</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>288</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -3301,7 +3347,7 @@
         <v>4</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
@@ -3320,7 +3366,7 @@
     <row r="29" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -3347,7 +3393,7 @@
     <row r="30" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10"/>
       <c r="B30" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -3374,7 +3420,7 @@
     <row r="31" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10"/>
       <c r="B31" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -3401,7 +3447,7 @@
     <row r="32" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -3428,7 +3474,7 @@
     <row r="33" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -3455,7 +3501,7 @@
     <row r="34" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10"/>
       <c r="B34" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -3481,17 +3527,17 @@
     </row>
     <row r="35" spans="1:19" s="17" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>61</v>
@@ -3509,20 +3555,20 @@
       <c r="O35" s="16"/>
       <c r="P35" s="16"/>
       <c r="Q35" s="16" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="R35" s="16"/>
       <c r="S35" s="16"/>
     </row>
     <row r="36" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="15" t="s">
@@ -3538,13 +3584,13 @@
     </row>
     <row r="37" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>599</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>600</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>601</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>602</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="15" t="s">
@@ -3560,7 +3606,7 @@
     </row>
     <row r="38" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>4</v>
@@ -3583,10 +3629,10 @@
     <row r="39" spans="1:19" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>296</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>297</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -3612,10 +3658,10 @@
     <row r="40" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -3625,7 +3671,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -3643,10 +3689,10 @@
     <row r="41" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -3672,10 +3718,10 @@
     <row r="42" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10"/>
       <c r="B42" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10" t="s">
@@ -3703,7 +3749,7 @@
     <row r="43" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -3730,17 +3776,17 @@
     <row r="44" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="10"/>
       <c r="B44" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>541</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>542</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>4</v>
@@ -3763,17 +3809,17 @@
     <row r="45" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>4</v>
@@ -3796,7 +3842,7 @@
     <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10"/>
       <c r="B46" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
@@ -3823,7 +3869,7 @@
     <row r="47" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10"/>
       <c r="B47" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
@@ -3850,7 +3896,7 @@
     <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10"/>
       <c r="B48" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -3877,7 +3923,7 @@
     <row r="49" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10"/>
       <c r="B49" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
@@ -3904,7 +3950,7 @@
     <row r="50" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10"/>
       <c r="B50" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -3931,7 +3977,7 @@
     <row r="51" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="10"/>
       <c r="B51" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -3958,7 +4004,7 @@
     <row r="52" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>
       <c r="B52" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -3985,7 +4031,7 @@
     <row r="53" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -4012,7 +4058,7 @@
     <row r="54" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -4039,7 +4085,7 @@
     <row r="55" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10"/>
       <c r="B55" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -4066,7 +4112,7 @@
     <row r="56" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
       <c r="B56" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -4093,7 +4139,7 @@
     <row r="57" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10"/>
       <c r="B57" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -4120,7 +4166,7 @@
     <row r="58" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10"/>
       <c r="B58" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -4147,7 +4193,7 @@
     <row r="59" spans="1:19" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A59" s="10"/>
       <c r="B59" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -4158,7 +4204,7 @@
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J59" s="10"/>
       <c r="K59" s="10"/>
@@ -4176,7 +4222,7 @@
     <row r="60" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10"/>
       <c r="B60" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -4203,7 +4249,7 @@
     <row r="61" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10"/>
       <c r="B61" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -4230,7 +4276,7 @@
     <row r="62" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -4257,7 +4303,7 @@
     <row r="63" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="10"/>
       <c r="B63" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -4284,7 +4330,7 @@
     <row r="64" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10"/>
       <c r="B64" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
@@ -4311,7 +4357,7 @@
     <row r="65" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10"/>
       <c r="B65" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -4338,7 +4384,7 @@
     <row r="66" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10"/>
       <c r="B66" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
@@ -4364,7 +4410,7 @@
     </row>
     <row r="67" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B67" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G67" s="12" t="s">
         <v>4</v>
@@ -4380,7 +4426,7 @@
     </row>
     <row r="68" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B68" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G68" s="12" t="s">
         <v>4</v>
@@ -4397,7 +4443,7 @@
     <row r="69" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10"/>
       <c r="B69" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -4423,7 +4469,7 @@
     </row>
     <row r="70" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B70" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G70" s="12" t="s">
         <v>4</v>
@@ -4440,7 +4486,7 @@
     <row r="71" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="10"/>
       <c r="B71" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
@@ -4467,7 +4513,7 @@
     <row r="72" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="10"/>
       <c r="B72" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -4494,7 +4540,7 @@
     <row r="73" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10"/>
       <c r="B73" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
@@ -4521,7 +4567,7 @@
     <row r="74" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="10"/>
       <c r="B74" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -4610,7 +4656,7 @@
     <row r="77" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="10"/>
       <c r="B77" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
@@ -4636,7 +4682,7 @@
     </row>
     <row r="78" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B78" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G78" s="12" t="s">
         <v>4</v>
@@ -4653,7 +4699,7 @@
     <row r="79" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="10"/>
       <c r="B79" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
@@ -4680,7 +4726,7 @@
     <row r="80" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="10"/>
       <c r="B80" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="21"/>
@@ -4710,7 +4756,7 @@
         <v>111</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D81" s="10"/>
       <c r="E81" s="11" t="s">
@@ -4738,10 +4784,10 @@
     <row r="82" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="10"/>
       <c r="B82" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C82" s="10" t="s">
         <v>281</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>282</v>
       </c>
       <c r="D82" s="10"/>
       <c r="E82" s="10"/>
@@ -4750,10 +4796,10 @@
         <v>4</v>
       </c>
       <c r="H82" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="I82" s="10" t="s">
         <v>334</v>
-      </c>
-      <c r="I82" s="10" t="s">
-        <v>335</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -4771,10 +4817,10 @@
     <row r="83" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="10"/>
       <c r="B83" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F83" s="10"/>
       <c r="G83" s="10" t="s">
@@ -4796,7 +4842,7 @@
     <row r="84" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="10"/>
       <c r="B84" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
@@ -4823,7 +4869,7 @@
     <row r="85" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="10"/>
       <c r="B85" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
@@ -4850,7 +4896,7 @@
     <row r="86" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10"/>
       <c r="B86" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
@@ -4877,12 +4923,12 @@
     <row r="87" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="10"/>
       <c r="B87" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
       <c r="E87" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F87" s="10"/>
       <c r="G87" s="10" t="s">
@@ -4906,7 +4952,7 @@
     <row r="88" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="10"/>
       <c r="B88" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
@@ -4931,7 +4977,7 @@
     <row r="89" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="10"/>
       <c r="B89" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
@@ -4982,10 +5028,10 @@
     </row>
     <row r="91" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B91" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G91" s="12" t="s">
         <v>4</v>
@@ -4999,7 +5045,7 @@
     </row>
     <row r="92" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B92" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>4</v>
@@ -5016,7 +5062,7 @@
     <row r="93" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="10"/>
       <c r="B93" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
@@ -5043,19 +5089,19 @@
     <row r="94" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="10"/>
       <c r="B94" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C94" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C94" s="12" t="s">
+      <c r="F94" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J94" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="F94" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G94" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J94" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="K94" s="13"/>
       <c r="O94" s="12">
@@ -5068,13 +5114,13 @@
     </row>
     <row r="95" spans="1:19" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B95" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C95" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C95" s="12" t="s">
-        <v>151</v>
-      </c>
       <c r="F95" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>4</v>
@@ -5091,7 +5137,7 @@
     <row r="96" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="10"/>
       <c r="B96" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
@@ -5118,7 +5164,7 @@
     <row r="97" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="10"/>
       <c r="B97" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
@@ -5145,7 +5191,7 @@
     <row r="98" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="10"/>
       <c r="B98" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
@@ -5172,7 +5218,7 @@
     <row r="99" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10"/>
       <c r="B99" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C99" s="10"/>
       <c r="D99" s="10"/>
@@ -5199,7 +5245,7 @@
     <row r="100" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="10"/>
       <c r="B100" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10"/>
@@ -5226,7 +5272,7 @@
     <row r="101" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10"/>
       <c r="B101" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
@@ -5253,7 +5299,7 @@
     <row r="102" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="10"/>
       <c r="B102" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
@@ -5280,7 +5326,7 @@
     <row r="103" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="10"/>
       <c r="B103" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C103" s="10"/>
       <c r="D103" s="10"/>
@@ -5307,7 +5353,7 @@
     <row r="104" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="10"/>
       <c r="B104" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="10"/>
@@ -5334,7 +5380,7 @@
     <row r="105" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10"/>
       <c r="B105" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C105" s="10"/>
       <c r="D105" s="10"/>
@@ -5361,7 +5407,7 @@
     <row r="106" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10"/>
       <c r="B106" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10"/>
@@ -5388,10 +5434,10 @@
     <row r="107" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="10"/>
       <c r="B107" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C107" s="10" t="s">
         <v>356</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>357</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="10"/>
@@ -5414,35 +5460,38 @@
       <c r="R107" s="10"/>
       <c r="S107" s="10"/>
     </row>
-    <row r="108" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E108" s="10"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H108" s="10"/>
-      <c r="I108" s="10"/>
-      <c r="J108" s="10"/>
-      <c r="K108" s="10"/>
-      <c r="L108" s="10"/>
-      <c r="M108" s="10"/>
-      <c r="N108" s="10"/>
-      <c r="O108" s="10"/>
-      <c r="P108" s="10"/>
-      <c r="Q108" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R108" s="10"/>
-      <c r="S108" s="10"/>
+    <row r="108" spans="1:20" s="25" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A108" s="23"/>
+      <c r="B108" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="C108" s="25" t="s">
+        <v>626</v>
+      </c>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H108" s="23"/>
+      <c r="I108" s="23"/>
+      <c r="J108" s="23"/>
+      <c r="K108" s="23"/>
+      <c r="L108" s="23"/>
+      <c r="M108" s="23"/>
+      <c r="N108" s="23"/>
+      <c r="O108" s="23"/>
+      <c r="P108" s="23"/>
+      <c r="Q108" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="R108" s="23"/>
+      <c r="S108" s="23"/>
     </row>
     <row r="109" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="10"/>
       <c r="B109" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="10"/>
@@ -5454,7 +5503,7 @@
       <c r="H109" s="10"/>
       <c r="I109" s="10"/>
       <c r="J109" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K109" s="10"/>
       <c r="L109" s="10"/>
@@ -5471,7 +5520,7 @@
     <row r="110" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="10"/>
       <c r="B110" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="10"/>
@@ -5497,7 +5546,7 @@
     <row r="111" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="10"/>
       <c r="B111" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C111" s="10"/>
       <c r="D111" s="10"/>
@@ -5524,7 +5573,7 @@
     <row r="112" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="10"/>
       <c r="B112" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C112" s="10"/>
       <c r="D112" s="10"/>
@@ -5552,7 +5601,7 @@
     <row r="113" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="10"/>
       <c r="B113" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="10"/>
@@ -5580,7 +5629,7 @@
     <row r="114" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10"/>
       <c r="B114" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="10"/>
@@ -5608,14 +5657,14 @@
     <row r="115" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="10"/>
       <c r="B115" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D115" s="10"/>
       <c r="E115" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F115" s="10"/>
       <c r="G115" s="10" t="s">
@@ -5640,7 +5689,7 @@
     <row r="116" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" s="10"/>
       <c r="B116" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C116" s="10"/>
       <c r="D116" s="10"/>
@@ -5668,7 +5717,7 @@
     <row r="117" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="10"/>
       <c r="B117" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C117" s="10"/>
       <c r="D117" s="10"/>
@@ -5696,7 +5745,7 @@
     <row r="118" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="10"/>
       <c r="B118" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C118" s="10"/>
       <c r="D118" s="10"/>
@@ -5724,7 +5773,7 @@
     <row r="119" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" s="10"/>
       <c r="B119" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C119" s="10"/>
       <c r="D119" s="10"/>
@@ -5752,7 +5801,7 @@
     <row r="120" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="10"/>
       <c r="B120" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C120" s="10"/>
       <c r="D120" s="10"/>
@@ -5779,10 +5828,10 @@
     </row>
     <row r="121" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B121" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C121" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="C121" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="G121" s="12" t="s">
         <v>4</v>
@@ -5799,10 +5848,10 @@
     </row>
     <row r="122" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B122" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C122" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>156</v>
       </c>
       <c r="G122" s="12" t="s">
         <v>4</v>
@@ -5819,17 +5868,17 @@
     </row>
     <row r="123" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B123" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D123" s="10"/>
       <c r="G123" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J123" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K123" s="13"/>
       <c r="O123" s="12">
@@ -5844,7 +5893,7 @@
     <row r="124" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A124" s="10"/>
       <c r="B124" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E124" s="10"/>
       <c r="F124" s="10"/>
@@ -5853,7 +5902,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -5872,7 +5921,7 @@
     <row r="125" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="10"/>
       <c r="B125" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C125" s="10"/>
       <c r="D125" s="10"/>
@@ -5900,7 +5949,7 @@
     <row r="126" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" s="10"/>
       <c r="B126" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C126" s="10"/>
       <c r="D126" s="10"/>
@@ -5927,7 +5976,7 @@
     </row>
     <row r="127" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B127" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G127" s="12" t="s">
         <v>4</v>
@@ -5944,13 +5993,13 @@
     </row>
     <row r="128" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B128" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G128" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J128" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K128" s="13"/>
       <c r="O128" s="12">
@@ -5964,7 +6013,7 @@
     </row>
     <row r="129" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B129" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>4</v>
@@ -5981,7 +6030,7 @@
     </row>
     <row r="130" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B130" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G130" s="12" t="s">
         <v>4</v>
@@ -5998,7 +6047,7 @@
     </row>
     <row r="131" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B131" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G131" s="12" t="s">
         <v>4</v>
@@ -6015,7 +6064,7 @@
     </row>
     <row r="132" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B132" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G132" s="12" t="s">
         <v>4</v>
@@ -6032,7 +6081,7 @@
     </row>
     <row r="133" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B133" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G133" s="12" t="s">
         <v>4</v>
@@ -6049,7 +6098,7 @@
     </row>
     <row r="134" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B134" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G134" s="12" t="s">
         <v>4</v>
@@ -6066,7 +6115,7 @@
     </row>
     <row r="135" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B135" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G135" s="12" t="s">
         <v>4</v>
@@ -6083,7 +6132,7 @@
     </row>
     <row r="136" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B136" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G136" s="12" t="s">
         <v>4</v>
@@ -6100,7 +6149,7 @@
     </row>
     <row r="137" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B137" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>4</v>
@@ -6117,7 +6166,7 @@
     </row>
     <row r="138" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B138" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G138" s="12" t="s">
         <v>4</v>
@@ -6134,7 +6183,7 @@
     </row>
     <row r="139" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B139" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G139" s="12" t="s">
         <v>4</v>
@@ -6151,7 +6200,7 @@
     </row>
     <row r="140" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B140" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G140" s="12" t="s">
         <v>4</v>
@@ -6169,7 +6218,7 @@
     <row r="141" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A141" s="10"/>
       <c r="B141" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C141" s="10"/>
       <c r="D141" s="10"/>
@@ -6197,7 +6246,7 @@
     <row r="142" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A142" s="10"/>
       <c r="B142" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C142" s="10"/>
       <c r="D142" s="10"/>
@@ -6225,7 +6274,7 @@
     <row r="143" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" s="10"/>
       <c r="B143" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
@@ -6252,7 +6301,7 @@
     </row>
     <row r="144" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B144" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G144" s="12" t="s">
         <v>4</v>
@@ -6270,7 +6319,7 @@
     <row r="145" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A145" s="10"/>
       <c r="B145" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
@@ -6298,7 +6347,7 @@
     <row r="146" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="10"/>
       <c r="B146" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
@@ -6326,10 +6375,10 @@
     <row r="147" spans="1:20" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A147" s="10"/>
       <c r="B147" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="C147" s="10" t="s">
         <v>381</v>
-      </c>
-      <c r="C147" s="10" t="s">
-        <v>382</v>
       </c>
       <c r="D147" s="10"/>
       <c r="E147" s="10"/>
@@ -6338,7 +6387,7 @@
         <v>4</v>
       </c>
       <c r="H147" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I147" s="10"/>
       <c r="J147" s="10"/>
@@ -6358,7 +6407,7 @@
     <row r="148" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A148" s="10"/>
       <c r="B148" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
@@ -6384,7 +6433,7 @@
     <row r="149" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="10"/>
       <c r="B149" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
@@ -6412,7 +6461,7 @@
     <row r="150" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="10"/>
       <c r="B150" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C150" s="10"/>
       <c r="D150" s="10"/>
@@ -6440,7 +6489,7 @@
     <row r="151" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="10"/>
       <c r="B151" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10"/>
@@ -6468,7 +6517,7 @@
     <row r="152" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="10"/>
       <c r="B152" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
@@ -6496,7 +6545,7 @@
     <row r="153" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="10"/>
       <c r="B153" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C153" s="10"/>
       <c r="D153" s="10"/>
@@ -6524,7 +6573,7 @@
     <row r="154" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A154" s="10"/>
       <c r="B154" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10"/>
@@ -6551,7 +6600,7 @@
     </row>
     <row r="155" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B155" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G155" s="12" t="s">
         <v>4</v>
@@ -6569,14 +6618,14 @@
     <row r="156" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A156" s="10"/>
       <c r="B156" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="C156" s="10" t="s">
         <v>391</v>
-      </c>
-      <c r="C156" s="10" t="s">
-        <v>392</v>
       </c>
       <c r="D156" s="10"/>
       <c r="E156" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F156" s="10"/>
       <c r="G156" s="10" t="s">
@@ -6603,7 +6652,7 @@
     <row r="157" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A157" s="10"/>
       <c r="B157" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E157" s="10"/>
       <c r="F157" s="10"/>
@@ -6628,7 +6677,7 @@
     </row>
     <row r="158" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B158" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G158" s="12" t="s">
         <v>4</v>
@@ -6649,7 +6698,7 @@
     <row r="159" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A159" s="10"/>
       <c r="B159" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C159" s="10"/>
       <c r="D159" s="10"/>
@@ -6677,7 +6726,7 @@
     <row r="160" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A160" s="10"/>
       <c r="B160" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C160" s="10"/>
       <c r="D160" s="10"/>
@@ -6689,7 +6738,7 @@
       <c r="H160" s="10"/>
       <c r="I160" s="10"/>
       <c r="J160" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K160" s="10"/>
       <c r="L160" s="10"/>
@@ -6707,7 +6756,7 @@
     <row r="161" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A161" s="10"/>
       <c r="B161" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C161" s="10"/>
       <c r="D161" s="10"/>
@@ -6735,7 +6784,7 @@
     <row r="162" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A162" s="10"/>
       <c r="B162" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C162" s="10"/>
       <c r="D162" s="10"/>
@@ -6763,7 +6812,7 @@
     <row r="163" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A163" s="10"/>
       <c r="B163" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C163" s="10"/>
       <c r="D163" s="10"/>
@@ -6791,7 +6840,7 @@
     <row r="164" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A164" s="10"/>
       <c r="B164" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C164" s="10"/>
       <c r="D164" s="10"/>
@@ -6819,7 +6868,7 @@
     <row r="165" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A165" s="10"/>
       <c r="B165" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C165" s="10"/>
       <c r="D165" s="10"/>
@@ -6847,7 +6896,7 @@
     <row r="166" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A166" s="10"/>
       <c r="B166" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
@@ -6875,7 +6924,7 @@
     <row r="167" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A167" s="10"/>
       <c r="B167" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C167" s="10"/>
       <c r="D167" s="10"/>
@@ -6903,7 +6952,7 @@
     <row r="168" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A168" s="10"/>
       <c r="B168" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C168" s="10"/>
       <c r="D168" s="10"/>
@@ -6931,7 +6980,7 @@
     <row r="169" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A169" s="10"/>
       <c r="B169" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
@@ -6959,7 +7008,7 @@
     <row r="170" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A170" s="10"/>
       <c r="B170" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C170" s="10"/>
       <c r="D170" s="10"/>
@@ -6987,7 +7036,7 @@
     <row r="171" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A171" s="10"/>
       <c r="B171" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
@@ -7015,7 +7064,7 @@
     <row r="172" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A172" s="10"/>
       <c r="B172" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
@@ -7043,7 +7092,7 @@
     <row r="173" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A173" s="10"/>
       <c r="B173" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
@@ -7055,7 +7104,7 @@
       <c r="H173" s="10"/>
       <c r="I173" s="10"/>
       <c r="J173" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K173" s="10"/>
       <c r="L173" s="10"/>
@@ -7073,10 +7122,10 @@
     <row r="174" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="10"/>
       <c r="B174" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C174" s="10" t="s">
         <v>409</v>
-      </c>
-      <c r="C174" s="10" t="s">
-        <v>410</v>
       </c>
       <c r="D174" s="10"/>
       <c r="E174" s="10"/>
@@ -7086,7 +7135,7 @@
       </c>
       <c r="H174" s="10"/>
       <c r="I174" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J174" s="10"/>
       <c r="K174" s="10"/>
@@ -7105,7 +7154,7 @@
     <row r="175" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A175" s="10"/>
       <c r="B175" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10"/>
@@ -7133,7 +7182,7 @@
     <row r="176" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A176" s="10"/>
       <c r="B176" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C176" s="10"/>
       <c r="D176" s="10"/>
@@ -7161,10 +7210,10 @@
     <row r="177" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A177" s="10"/>
       <c r="B177" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="C177" s="10" t="s">
         <v>414</v>
-      </c>
-      <c r="C177" s="10" t="s">
-        <v>415</v>
       </c>
       <c r="D177" s="10"/>
       <c r="E177" s="10" t="s">
@@ -7226,7 +7275,7 @@
     </row>
     <row r="179" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B179" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G179" s="12" t="s">
         <v>4</v>
@@ -7243,7 +7292,7 @@
     </row>
     <row r="180" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B180" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G180" s="12" t="s">
         <v>4</v>
@@ -7261,7 +7310,7 @@
     <row r="181" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A181" s="10"/>
       <c r="B181" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C181" s="10"/>
       <c r="D181" s="10"/>
@@ -7288,7 +7337,7 @@
     </row>
     <row r="182" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B182" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G182" s="12" t="s">
         <v>4</v>
@@ -7306,7 +7355,7 @@
     <row r="183" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A183" s="10"/>
       <c r="B183" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C183" s="10"/>
       <c r="D183" s="10"/>
@@ -7334,7 +7383,7 @@
     <row r="184" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A184" s="10"/>
       <c r="B184" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C184" s="10"/>
       <c r="D184" s="10"/>
@@ -7362,7 +7411,7 @@
     <row r="185" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A185" s="10"/>
       <c r="B185" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C185" s="10"/>
       <c r="D185" s="10"/>
@@ -7390,7 +7439,7 @@
     <row r="186" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A186" s="10"/>
       <c r="B186" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C186" s="10"/>
       <c r="D186" s="10"/>
@@ -7417,7 +7466,7 @@
     </row>
     <row r="187" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B187" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G187" s="12" t="s">
         <v>4</v>
@@ -7435,7 +7484,7 @@
     <row r="188" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A188" s="10"/>
       <c r="B188" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C188" s="10"/>
       <c r="D188" s="10"/>
@@ -7463,7 +7512,7 @@
     <row r="189" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A189" s="10"/>
       <c r="B189" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C189" s="10"/>
       <c r="D189" s="10"/>
@@ -7491,7 +7540,7 @@
     <row r="190" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A190" s="10"/>
       <c r="B190" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C190" s="10"/>
       <c r="D190" s="10"/>
@@ -7519,7 +7568,7 @@
     <row r="191" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A191" s="10"/>
       <c r="B191" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C191" s="10"/>
       <c r="D191" s="10"/>
@@ -7547,7 +7596,7 @@
     <row r="192" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A192" s="10"/>
       <c r="B192" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C192" s="10"/>
       <c r="D192" s="10"/>
@@ -7575,7 +7624,7 @@
     <row r="193" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A193" s="10"/>
       <c r="B193" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C193" s="10"/>
       <c r="D193" s="10"/>
@@ -7602,7 +7651,7 @@
     </row>
     <row r="194" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B194" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G194" s="12" t="s">
         <v>4</v>
@@ -7620,7 +7669,7 @@
     <row r="195" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" s="10"/>
       <c r="B195" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C195" s="10"/>
       <c r="D195" s="10"/>
@@ -7647,7 +7696,7 @@
     </row>
     <row r="196" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B196" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G196" s="12" t="s">
         <v>4</v>
@@ -7664,7 +7713,7 @@
     </row>
     <row r="197" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B197" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G197" s="12" t="s">
         <v>4</v>
@@ -7681,7 +7730,7 @@
     </row>
     <row r="198" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B198" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G198" s="12" t="s">
         <v>4</v>
@@ -7698,7 +7747,7 @@
     </row>
     <row r="199" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B199" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G199" s="12" t="s">
         <v>4</v>
@@ -7715,7 +7764,7 @@
     </row>
     <row r="200" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B200" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G200" s="12" t="s">
         <v>4</v>
@@ -7732,7 +7781,7 @@
     </row>
     <row r="201" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B201" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G201" s="12" t="s">
         <v>4</v>
@@ -7750,7 +7799,7 @@
     <row r="202" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A202" s="10"/>
       <c r="B202" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C202" s="10"/>
       <c r="D202" s="10"/>
@@ -7777,7 +7826,7 @@
     </row>
     <row r="203" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B203" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G203" s="12" t="s">
         <v>4</v>
@@ -7795,7 +7844,7 @@
     <row r="204" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A204" s="10"/>
       <c r="B204" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C204" s="10"/>
       <c r="D204" s="10"/>
@@ -7823,7 +7872,7 @@
     <row r="205" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A205" s="10"/>
       <c r="B205" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C205" s="10"/>
       <c r="D205" s="10"/>
@@ -7851,7 +7900,7 @@
     <row r="206" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A206" s="10"/>
       <c r="B206" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C206" s="10"/>
       <c r="D206" s="10"/>
@@ -7879,7 +7928,7 @@
     <row r="207" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A207" s="10"/>
       <c r="B207" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C207" s="10"/>
       <c r="D207" s="10"/>
@@ -7906,7 +7955,7 @@
     </row>
     <row r="208" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B208" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G208" s="12" t="s">
         <v>4</v>
@@ -7923,13 +7972,13 @@
     </row>
     <row r="209" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B209" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="G209" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J209" s="12" t="s">
         <v>190</v>
-      </c>
-      <c r="G209" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J209" s="12" t="s">
-        <v>191</v>
       </c>
       <c r="K209" s="13"/>
       <c r="O209" s="12">
@@ -7944,7 +7993,7 @@
     <row r="210" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A210" s="10"/>
       <c r="B210" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C210" s="10"/>
       <c r="D210" s="10"/>
@@ -7972,7 +8021,7 @@
     <row r="211" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A211" s="10"/>
       <c r="B211" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C211" s="10"/>
       <c r="D211" s="10"/>
@@ -8000,7 +8049,7 @@
     <row r="212" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A212" s="10"/>
       <c r="B212" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C212" s="10"/>
       <c r="D212" s="10"/>
@@ -8028,7 +8077,7 @@
     <row r="213" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A213" s="10"/>
       <c r="B213" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C213" s="10"/>
       <c r="D213" s="10"/>
@@ -8056,7 +8105,7 @@
     <row r="214" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A214" s="10"/>
       <c r="B214" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C214" s="10"/>
       <c r="D214" s="10"/>
@@ -8084,7 +8133,7 @@
     <row r="215" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A215" s="10"/>
       <c r="B215" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C215" s="10"/>
       <c r="D215" s="10"/>
@@ -8111,7 +8160,7 @@
     </row>
     <row r="216" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B216" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G216" s="12" t="s">
         <v>4</v>
@@ -8129,7 +8178,7 @@
     <row r="217" spans="1:20" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A217" s="10"/>
       <c r="B217" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C217" s="10"/>
       <c r="D217" s="10"/>
@@ -8157,7 +8206,7 @@
     <row r="218" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="10"/>
       <c r="B218" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C218" s="10"/>
       <c r="D218" s="10"/>
@@ -8185,7 +8234,7 @@
     <row r="219" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="10"/>
       <c r="B219" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C219" s="10"/>
       <c r="D219" s="10"/>
@@ -8197,7 +8246,7 @@
       <c r="H219" s="10"/>
       <c r="I219" s="10"/>
       <c r="J219" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K219" s="10"/>
       <c r="L219" s="10"/>
@@ -8215,7 +8264,7 @@
     <row r="220" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A220" s="10"/>
       <c r="B220" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C220" s="10"/>
       <c r="D220" s="10"/>
@@ -8242,7 +8291,7 @@
     </row>
     <row r="221" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B221" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G221" s="12" t="s">
         <v>4</v>
@@ -8260,7 +8309,7 @@
     <row r="222" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A222" s="10"/>
       <c r="B222" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C222" s="10"/>
       <c r="D222" s="10"/>
@@ -8288,7 +8337,7 @@
     <row r="223" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A223" s="10"/>
       <c r="B223" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C223" s="10"/>
       <c r="D223" s="10"/>
@@ -8316,7 +8365,7 @@
     <row r="224" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A224" s="10"/>
       <c r="B224" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C224" s="10"/>
       <c r="D224" s="10"/>
@@ -8344,7 +8393,7 @@
     <row r="225" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A225" s="10"/>
       <c r="B225" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C225" s="10"/>
       <c r="D225" s="10"/>
@@ -8400,7 +8449,7 @@
     <row r="227" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A227" s="10"/>
       <c r="B227" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C227" s="10"/>
       <c r="D227" s="10"/>
@@ -8428,7 +8477,7 @@
     <row r="228" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A228" s="10"/>
       <c r="B228" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C228" s="10"/>
       <c r="D228" s="10"/>
@@ -8456,7 +8505,7 @@
     <row r="229" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A229" s="10"/>
       <c r="B229" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C229" s="10"/>
       <c r="D229" s="10"/>
@@ -8484,7 +8533,7 @@
     <row r="230" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A230" s="10"/>
       <c r="B230" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C230" s="10"/>
       <c r="D230" s="10"/>
@@ -8512,7 +8561,7 @@
     <row r="231" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A231" s="10"/>
       <c r="B231" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C231" s="10"/>
       <c r="D231" s="10"/>
@@ -8540,7 +8589,7 @@
     <row r="232" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A232" s="10"/>
       <c r="B232" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C232" s="10"/>
       <c r="D232" s="10"/>
@@ -8567,7 +8616,7 @@
     </row>
     <row r="233" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B233" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G233" s="12" t="s">
         <v>4</v>
@@ -8584,7 +8633,7 @@
     </row>
     <row r="234" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B234" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G234" s="12" t="s">
         <v>4</v>
@@ -8601,10 +8650,10 @@
     </row>
     <row r="235" spans="1:20" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B235" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C235" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="C235" s="12" t="s">
-        <v>197</v>
       </c>
       <c r="G235" s="12" t="s">
         <v>4</v>
@@ -8621,7 +8670,7 @@
     </row>
     <row r="236" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B236" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G236" s="12" t="s">
         <v>4</v>
@@ -8639,7 +8688,7 @@
     <row r="237" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A237" s="10"/>
       <c r="B237" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C237" s="10"/>
       <c r="D237" s="10"/>
@@ -8667,7 +8716,7 @@
     <row r="238" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A238" s="10"/>
       <c r="B238" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C238" s="10"/>
       <c r="D238" s="10"/>
@@ -8695,7 +8744,7 @@
     <row r="239" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A239" s="10"/>
       <c r="B239" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C239" s="10"/>
       <c r="D239" s="10"/>
@@ -8723,7 +8772,7 @@
     <row r="240" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A240" s="10"/>
       <c r="B240" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C240" s="10"/>
       <c r="D240" s="10"/>
@@ -8751,7 +8800,7 @@
     <row r="241" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A241" s="10"/>
       <c r="B241" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C241" s="10"/>
       <c r="D241" s="10"/>
@@ -8779,7 +8828,7 @@
     <row r="242" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A242" s="10"/>
       <c r="B242" s="10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C242" s="10"/>
       <c r="D242" s="10"/>
@@ -8807,7 +8856,7 @@
     <row r="243" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A243" s="10"/>
       <c r="B243" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C243" s="10"/>
       <c r="D243" s="10"/>
@@ -8835,7 +8884,7 @@
     <row r="244" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A244" s="10"/>
       <c r="B244" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C244" s="10"/>
       <c r="D244" s="10"/>
@@ -8863,7 +8912,7 @@
     <row r="245" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A245" s="10"/>
       <c r="B245" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C245" s="10"/>
       <c r="D245" s="10"/>
@@ -8891,7 +8940,7 @@
     <row r="246" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A246" s="10"/>
       <c r="B246" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C246" s="10"/>
       <c r="D246" s="10"/>
@@ -8903,7 +8952,7 @@
       <c r="H246" s="10"/>
       <c r="I246" s="10"/>
       <c r="J246" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K246" s="10"/>
       <c r="L246" s="10"/>
@@ -8921,7 +8970,7 @@
     <row r="247" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A247" s="10"/>
       <c r="B247" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C247" s="10"/>
       <c r="D247" s="10"/>
@@ -8949,7 +8998,7 @@
     <row r="248" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A248" s="10"/>
       <c r="B248" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C248" s="10"/>
       <c r="D248" s="10"/>
@@ -8977,7 +9026,7 @@
     <row r="249" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A249" s="10"/>
       <c r="B249" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C249" s="10"/>
       <c r="D249" s="10"/>
@@ -9005,7 +9054,7 @@
     <row r="250" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A250" s="10"/>
       <c r="B250" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C250" s="10"/>
       <c r="D250" s="10"/>
@@ -9033,10 +9082,10 @@
     <row r="251" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A251" s="10"/>
       <c r="B251" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="C251" s="10" t="s">
         <v>469</v>
-      </c>
-      <c r="C251" s="10" t="s">
-        <v>470</v>
       </c>
       <c r="D251" s="10"/>
       <c r="E251" s="10"/>
@@ -9063,7 +9112,7 @@
     <row r="252" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A252" s="10"/>
       <c r="B252" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C252" s="10"/>
       <c r="D252" s="10"/>
@@ -9091,7 +9140,7 @@
     <row r="253" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A253" s="10"/>
       <c r="B253" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C253" s="10"/>
       <c r="D253" s="10"/>
@@ -9119,7 +9168,7 @@
     <row r="254" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A254" s="10"/>
       <c r="B254" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C254" s="10"/>
       <c r="D254" s="10"/>
@@ -9147,7 +9196,7 @@
     <row r="255" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A255" s="10"/>
       <c r="B255" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C255" s="10"/>
       <c r="D255" s="10"/>
@@ -9175,7 +9224,7 @@
     <row r="256" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A256" s="10"/>
       <c r="B256" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C256" s="10"/>
       <c r="D256" s="10"/>
@@ -9203,10 +9252,10 @@
     <row r="257" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A257" s="10"/>
       <c r="B257" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C257" s="10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D257" s="10"/>
       <c r="E257" s="10" t="s">
@@ -9235,7 +9284,7 @@
         <v>126</v>
       </c>
       <c r="C258" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G258" s="12" t="s">
         <v>4</v>
@@ -9252,7 +9301,7 @@
     </row>
     <row r="259" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B259" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G259" s="12" t="s">
         <v>4</v>
@@ -9270,7 +9319,7 @@
     <row r="260" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A260" s="10"/>
       <c r="B260" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C260" s="10"/>
       <c r="D260" s="10"/>
@@ -9298,7 +9347,7 @@
     <row r="261" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A261" s="10"/>
       <c r="B261" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C261" s="10"/>
       <c r="D261" s="10"/>
@@ -9326,7 +9375,7 @@
     <row r="262" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A262" s="10"/>
       <c r="B262" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C262" s="10"/>
       <c r="D262" s="10"/>
@@ -9354,7 +9403,7 @@
     <row r="263" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A263" s="10"/>
       <c r="B263" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C263" s="10"/>
       <c r="D263" s="10"/>
@@ -9382,7 +9431,7 @@
     <row r="264" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A264" s="10"/>
       <c r="B264" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C264" s="10"/>
       <c r="D264" s="10"/>
@@ -9436,7 +9485,7 @@
     <row r="266" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A266" s="10"/>
       <c r="B266" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C266" s="10"/>
       <c r="D266" s="10"/>
@@ -9464,7 +9513,7 @@
     <row r="267" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A267" s="10"/>
       <c r="B267" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C267" s="10"/>
       <c r="D267" s="10"/>
@@ -9492,7 +9541,7 @@
     <row r="268" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A268" s="10"/>
       <c r="B268" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C268" s="10"/>
       <c r="D268" s="10"/>
@@ -9520,7 +9569,7 @@
     <row r="269" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A269" s="10"/>
       <c r="B269" s="10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C269" s="10"/>
       <c r="D269" s="10"/>
@@ -9548,7 +9597,7 @@
     <row r="270" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A270" s="10"/>
       <c r="B270" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C270" s="10"/>
       <c r="D270" s="10"/>
@@ -9612,10 +9661,10 @@
     <row r="272" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A272" s="10"/>
       <c r="B272" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C272" s="10" t="s">
         <v>486</v>
-      </c>
-      <c r="C272" s="10" t="s">
-        <v>487</v>
       </c>
       <c r="D272" s="10"/>
       <c r="E272" s="10"/>
@@ -9625,7 +9674,7 @@
       </c>
       <c r="H272" s="10"/>
       <c r="I272" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J272" s="10"/>
       <c r="K272" s="10"/>
@@ -9644,7 +9693,7 @@
     <row r="273" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A273" s="10"/>
       <c r="B273" s="10" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C273" s="10"/>
       <c r="D273" s="10"/>
@@ -9671,7 +9720,7 @@
     </row>
     <row r="274" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B274" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G274" s="12" t="s">
         <v>4</v>
@@ -9688,7 +9737,7 @@
     </row>
     <row r="275" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B275" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G275" s="12" t="s">
         <v>4</v>
@@ -9705,10 +9754,10 @@
     </row>
     <row r="276" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B276" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C276" s="12" t="s">
         <v>203</v>
-      </c>
-      <c r="C276" s="12" t="s">
-        <v>204</v>
       </c>
       <c r="G276" s="12" t="s">
         <v>4</v>
@@ -9725,7 +9774,7 @@
     </row>
     <row r="277" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B277" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G277" s="12" t="s">
         <v>4</v>
@@ -9742,7 +9791,7 @@
     </row>
     <row r="278" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B278" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G278" s="12" t="s">
         <v>4</v>
@@ -9759,7 +9808,7 @@
     </row>
     <row r="279" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B279" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G279" s="12" t="s">
         <v>4</v>
@@ -9776,7 +9825,7 @@
     </row>
     <row r="280" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B280" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G280" s="12" t="s">
         <v>4</v>
@@ -9793,7 +9842,7 @@
     </row>
     <row r="281" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B281" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G281" s="12" t="s">
         <v>4</v>
@@ -9810,7 +9859,7 @@
     </row>
     <row r="282" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B282" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G282" s="12" t="s">
         <v>4</v>
@@ -9827,7 +9876,7 @@
     </row>
     <row r="283" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B283" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G283" s="12" t="s">
         <v>4</v>
@@ -9844,7 +9893,7 @@
     </row>
     <row r="284" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B284" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G284" s="12" t="s">
         <v>4</v>
@@ -9861,7 +9910,7 @@
     </row>
     <row r="285" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B285" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G285" s="12" t="s">
         <v>4</v>
@@ -9878,7 +9927,7 @@
     </row>
     <row r="286" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B286" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G286" s="12" t="s">
         <v>4</v>
@@ -9895,7 +9944,7 @@
     </row>
     <row r="287" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B287" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G287" s="12" t="s">
         <v>4</v>
@@ -9912,7 +9961,7 @@
     </row>
     <row r="288" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B288" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G288" s="12" t="s">
         <v>4</v>
@@ -9929,7 +9978,7 @@
     </row>
     <row r="289" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B289" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G289" s="12" t="s">
         <v>4</v>
@@ -9946,7 +9995,7 @@
     </row>
     <row r="290" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B290" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G290" s="12" t="s">
         <v>4</v>
@@ -9964,7 +10013,7 @@
     <row r="291" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A291" s="10"/>
       <c r="B291" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C291" s="10"/>
       <c r="D291" s="10"/>
@@ -9992,7 +10041,7 @@
     <row r="292" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A292" s="10"/>
       <c r="B292" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C292" s="10"/>
       <c r="D292" s="10"/>
@@ -10020,7 +10069,7 @@
     <row r="293" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A293" s="10"/>
       <c r="B293" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C293" s="10"/>
       <c r="D293" s="10"/>
@@ -10047,7 +10096,7 @@
     </row>
     <row r="294" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B294" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G294" s="12" t="s">
         <v>4</v>
@@ -10065,7 +10114,7 @@
     <row r="295" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A295" s="10"/>
       <c r="B295" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C295" s="10"/>
       <c r="D295" s="10"/>
@@ -10093,7 +10142,7 @@
     <row r="296" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A296" s="10"/>
       <c r="B296" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C296" s="10"/>
       <c r="D296" s="10"/>
@@ -10105,7 +10154,7 @@
       <c r="H296" s="10"/>
       <c r="I296" s="10"/>
       <c r="J296" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K296" s="10"/>
       <c r="L296" s="10"/>
@@ -10123,7 +10172,7 @@
     <row r="297" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A297" s="10"/>
       <c r="B297" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C297" s="10"/>
       <c r="D297" s="10"/>
@@ -10151,7 +10200,7 @@
     <row r="298" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A298" s="10"/>
       <c r="B298" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C298" s="10"/>
       <c r="D298" s="10"/>
@@ -10178,7 +10227,7 @@
     </row>
     <row r="299" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B299" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G299" s="12" t="s">
         <v>4</v>
@@ -10195,7 +10244,7 @@
     </row>
     <row r="300" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B300" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G300" s="12" t="s">
         <v>4</v>
@@ -10213,7 +10262,7 @@
     <row r="301" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A301" s="10"/>
       <c r="B301" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C301" s="10"/>
       <c r="D301" s="10"/>
@@ -10241,7 +10290,7 @@
     <row r="302" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A302" s="10"/>
       <c r="B302" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C302" s="10"/>
       <c r="D302" s="10"/>
@@ -10269,7 +10318,7 @@
     <row r="303" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A303" s="10"/>
       <c r="B303" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C303" s="10"/>
       <c r="D303" s="10"/>
@@ -10297,7 +10346,7 @@
     <row r="304" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A304" s="10"/>
       <c r="B304" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C304" s="10"/>
       <c r="D304" s="10"/>
@@ -10325,7 +10374,7 @@
     <row r="305" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A305" s="10"/>
       <c r="B305" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C305" s="10"/>
       <c r="D305" s="10"/>
@@ -10353,7 +10402,7 @@
     <row r="306" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A306" s="10"/>
       <c r="B306" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C306" s="10"/>
       <c r="D306" s="10"/>
@@ -10381,7 +10430,7 @@
     <row r="307" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A307" s="10"/>
       <c r="B307" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C307" s="10"/>
       <c r="D307" s="10"/>
@@ -10409,7 +10458,7 @@
     <row r="308" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A308" s="10"/>
       <c r="B308" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C308" s="10"/>
       <c r="D308" s="10"/>
@@ -10437,7 +10486,7 @@
     <row r="309" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A309" s="10"/>
       <c r="B309" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C309" s="10"/>
       <c r="D309" s="10"/>
@@ -10465,7 +10514,7 @@
     <row r="310" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A310" s="10"/>
       <c r="B310" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C310" s="10"/>
       <c r="D310" s="10"/>
@@ -10492,7 +10541,7 @@
     </row>
     <row r="311" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B311" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G311" s="12" t="s">
         <v>4</v>
@@ -10510,7 +10559,7 @@
     <row r="312" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A312" s="10"/>
       <c r="B312" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C312" s="10"/>
       <c r="D312" s="10"/>
@@ -10537,7 +10586,7 @@
     </row>
     <row r="313" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B313" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G313" s="12" t="s">
         <v>4</v>
@@ -10555,7 +10604,7 @@
     <row r="314" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A314" s="10"/>
       <c r="B314" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C314" s="10"/>
       <c r="D314" s="10"/>
@@ -10583,7 +10632,7 @@
     <row r="315" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A315" s="10"/>
       <c r="B315" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C315" s="10"/>
       <c r="D315" s="10"/>
@@ -10611,7 +10660,7 @@
     <row r="316" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A316" s="10"/>
       <c r="B316" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C316" s="10"/>
       <c r="D316" s="10"/>
@@ -10639,7 +10688,7 @@
     <row r="317" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A317" s="10"/>
       <c r="B317" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C317" s="10"/>
       <c r="D317" s="10"/>
@@ -10667,7 +10716,7 @@
     <row r="318" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A318" s="10"/>
       <c r="B318" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C318" s="10"/>
       <c r="D318" s="10"/>
@@ -10695,7 +10744,7 @@
     <row r="319" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A319" s="10"/>
       <c r="B319" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C319" s="10"/>
       <c r="D319" s="10"/>
@@ -10723,7 +10772,7 @@
     <row r="320" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A320" s="10"/>
       <c r="B320" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C320" s="10"/>
       <c r="D320" s="10"/>
@@ -10751,7 +10800,7 @@
     <row r="321" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A321" s="10"/>
       <c r="B321" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C321" s="10"/>
       <c r="D321" s="10"/>
@@ -10779,7 +10828,7 @@
     <row r="322" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A322" s="10"/>
       <c r="B322" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C322" s="10"/>
       <c r="D322" s="10"/>
@@ -10807,7 +10856,7 @@
     <row r="323" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A323" s="10"/>
       <c r="B323" s="10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C323" s="10"/>
       <c r="D323" s="10"/>
@@ -10834,7 +10883,7 @@
     </row>
     <row r="324" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B324" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G324" s="12" t="s">
         <v>4</v>
@@ -10851,7 +10900,7 @@
     </row>
     <row r="325" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B325" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G325" s="12" t="s">
         <v>4</v>
@@ -10869,7 +10918,7 @@
     <row r="326" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A326" s="10"/>
       <c r="B326" s="10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C326" s="10"/>
       <c r="D326" s="10"/>
@@ -10897,7 +10946,7 @@
     <row r="327" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A327" s="10"/>
       <c r="B327" s="10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C327" s="10"/>
       <c r="D327" s="10"/>
@@ -10930,7 +10979,7 @@
         <v>4</v>
       </c>
       <c r="J328" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K328" s="13"/>
       <c r="O328" s="12">
@@ -10944,13 +10993,13 @@
     </row>
     <row r="329" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B329" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G329" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J329" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K329" s="13"/>
       <c r="O329" s="12">
@@ -10964,7 +11013,7 @@
     </row>
     <row r="330" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B330" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G330" s="12" t="s">
         <v>4</v>
@@ -10981,13 +11030,13 @@
     </row>
     <row r="331" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B331" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G331" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J331" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K331" s="13"/>
       <c r="O331" s="12">
@@ -11001,7 +11050,7 @@
     </row>
     <row r="332" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B332" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G332" s="12" t="s">
         <v>4</v>
@@ -11018,7 +11067,7 @@
     </row>
     <row r="333" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B333" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G333" s="12" t="s">
         <v>4</v>
@@ -11035,7 +11084,7 @@
     </row>
     <row r="334" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B334" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G334" s="12" t="s">
         <v>4</v>
@@ -11069,7 +11118,7 @@
     </row>
     <row r="336" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B336" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G336" s="12" t="s">
         <v>4</v>
@@ -11086,7 +11135,7 @@
     </row>
     <row r="337" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B337" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G337" s="12" t="s">
         <v>4</v>
@@ -11104,7 +11153,7 @@
     <row r="338" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A338" s="10"/>
       <c r="B338" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C338" s="10"/>
       <c r="D338" s="10"/>
@@ -11132,7 +11181,7 @@
     <row r="339" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A339" s="10"/>
       <c r="B339" s="10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C339" s="10"/>
       <c r="D339" s="10"/>
@@ -11160,7 +11209,7 @@
     <row r="340" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A340" s="10"/>
       <c r="B340" s="10" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C340" s="10"/>
       <c r="D340" s="10"/>
@@ -11188,7 +11237,7 @@
     <row r="341" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A341" s="10"/>
       <c r="B341" s="10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C341" s="10"/>
       <c r="D341" s="10"/>
@@ -11216,7 +11265,7 @@
     <row r="342" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A342" s="10"/>
       <c r="B342" s="10" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C342" s="10"/>
       <c r="D342" s="10"/>
@@ -11244,7 +11293,7 @@
     <row r="343" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A343" s="10"/>
       <c r="B343" s="10" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C343" s="10"/>
       <c r="D343" s="10"/>
@@ -11269,68 +11318,71 @@
       <c r="S343" s="10"/>
       <c r="T343" s="10"/>
     </row>
-    <row r="344" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A344" s="10"/>
-      <c r="B344" s="10" t="s">
+    <row r="344" spans="1:20" s="25" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A344" s="23"/>
+      <c r="B344" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C344" s="11" t="s">
-        <v>582</v>
-      </c>
-      <c r="D344" s="21"/>
-      <c r="E344" s="10"/>
-      <c r="F344" s="10"/>
-      <c r="G344" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H344" s="10"/>
-      <c r="I344" s="10"/>
-      <c r="J344" s="10"/>
-      <c r="K344" s="10"/>
-      <c r="L344" s="10"/>
-      <c r="M344" s="10"/>
-      <c r="N344" s="10"/>
-      <c r="O344" s="10"/>
-      <c r="P344" s="10"/>
-      <c r="Q344" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R344" s="10"/>
-      <c r="S344" s="10"/>
-      <c r="T344" s="10"/>
-    </row>
-    <row r="345" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A345" s="10"/>
-      <c r="B345" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="C345" s="10"/>
-      <c r="D345" s="10"/>
-      <c r="E345" s="10"/>
-      <c r="F345" s="10"/>
-      <c r="G345" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H345" s="10"/>
-      <c r="I345" s="10"/>
-      <c r="J345" s="10"/>
-      <c r="K345" s="10"/>
-      <c r="L345" s="10"/>
-      <c r="M345" s="10"/>
-      <c r="N345" s="10"/>
-      <c r="O345" s="10"/>
-      <c r="P345" s="10"/>
-      <c r="Q345" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R345" s="10"/>
-      <c r="S345" s="10"/>
-      <c r="T345" s="10"/>
+      <c r="C344" s="26" t="s">
+        <v>620</v>
+      </c>
+      <c r="D344" s="27"/>
+      <c r="E344" s="23"/>
+      <c r="F344" s="23"/>
+      <c r="G344" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H344" s="23"/>
+      <c r="I344" s="23"/>
+      <c r="K344" s="23" t="s">
+        <v>621</v>
+      </c>
+      <c r="L344" s="23"/>
+      <c r="M344" s="23"/>
+      <c r="N344" s="23"/>
+      <c r="O344" s="23"/>
+      <c r="P344" s="23"/>
+      <c r="Q344" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="R344" s="23"/>
+      <c r="S344" s="23"/>
+      <c r="T344" s="23"/>
+    </row>
+    <row r="345" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A345" s="23"/>
+      <c r="B345" s="23" t="s">
+        <v>525</v>
+      </c>
+      <c r="C345" s="23" t="s">
+        <v>619</v>
+      </c>
+      <c r="D345" s="23"/>
+      <c r="E345" s="23"/>
+      <c r="F345" s="23"/>
+      <c r="G345" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H345" s="23"/>
+      <c r="I345" s="23"/>
+      <c r="J345" s="23"/>
+      <c r="K345" s="23"/>
+      <c r="L345" s="23"/>
+      <c r="M345" s="23"/>
+      <c r="N345" s="23"/>
+      <c r="O345" s="23"/>
+      <c r="P345" s="23"/>
+      <c r="Q345" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="R345" s="23"/>
+      <c r="S345" s="23"/>
+      <c r="T345" s="23"/>
     </row>
     <row r="346" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A346" s="10"/>
       <c r="B346" s="10" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C346" s="10"/>
       <c r="D346" s="10"/>
@@ -11358,7 +11410,7 @@
     <row r="347" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A347" s="10"/>
       <c r="B347" s="10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C347" s="10"/>
       <c r="D347" s="10"/>
@@ -11370,7 +11422,7 @@
       <c r="H347" s="10"/>
       <c r="I347" s="10"/>
       <c r="J347" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K347" s="10"/>
       <c r="L347" s="10"/>
@@ -11388,7 +11440,7 @@
     <row r="348" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A348" s="10"/>
       <c r="B348" s="10" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C348" s="10"/>
       <c r="D348" s="10"/>
@@ -11416,7 +11468,7 @@
     <row r="349" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A349" s="10"/>
       <c r="B349" s="10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C349" s="10"/>
       <c r="D349" s="10"/>
@@ -11444,10 +11496,10 @@
     <row r="350" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A350" s="10"/>
       <c r="B350" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="C350" s="10" t="s">
         <v>532</v>
-      </c>
-      <c r="C350" s="10" t="s">
-        <v>533</v>
       </c>
       <c r="D350" s="10"/>
       <c r="E350" s="10"/>
@@ -11474,7 +11526,7 @@
     <row r="351" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A351" s="10"/>
       <c r="B351" s="10" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C351" s="10"/>
       <c r="D351" s="10"/>
@@ -11502,10 +11554,10 @@
     <row r="352" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A352" s="10"/>
       <c r="B352" s="10" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C352" s="10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D352" s="10"/>
       <c r="E352" s="10"/>
@@ -11532,7 +11584,7 @@
     <row r="353" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A353" s="10"/>
       <c r="B353" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C353" s="10"/>
       <c r="D353" s="10"/>
@@ -11559,7 +11611,7 @@
     </row>
     <row r="354" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B354" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G354" s="12" t="s">
         <v>4</v>
@@ -11576,7 +11628,7 @@
     </row>
     <row r="355" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B355" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G355" s="12" t="s">
         <v>4</v>
@@ -11593,7 +11645,7 @@
     </row>
     <row r="356" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B356" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G356" s="12" t="s">
         <v>4</v>
@@ -11611,7 +11663,7 @@
     <row r="357" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A357" s="10"/>
       <c r="B357" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C357" s="10"/>
       <c r="D357" s="10"/>
@@ -11638,7 +11690,7 @@
     </row>
     <row r="358" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B358" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G358" s="12" t="s">
         <v>4</v>
@@ -11655,7 +11707,7 @@
     </row>
     <row r="359" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B359" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G359" s="12" t="s">
         <v>4</v>
@@ -11672,16 +11724,16 @@
     </row>
     <row r="360" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B360" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="C360" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C360" s="12" t="s">
+      <c r="E360" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="E360" s="12" t="s">
-        <v>242</v>
-      </c>
       <c r="F360" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G360" s="12" t="s">
         <v>4</v>
@@ -11699,7 +11751,7 @@
     <row r="361" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A361" s="10"/>
       <c r="B361" s="10" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C361" s="10"/>
       <c r="D361" s="10"/>
@@ -11726,7 +11778,7 @@
     </row>
     <row r="362" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B362" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G362" s="12" t="s">
         <v>4</v>
@@ -11743,13 +11795,13 @@
     </row>
     <row r="363" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B363" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C363" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="C363" s="12" t="s">
+      <c r="E363" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="E363" s="12" t="s">
-        <v>246</v>
       </c>
       <c r="F363" s="12" t="s">
         <v>69</v>
@@ -11769,7 +11821,7 @@
     </row>
     <row r="364" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B364" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G364" s="12" t="s">
         <v>4</v>
@@ -11786,13 +11838,13 @@
     </row>
     <row r="365" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B365" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C365" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="C365" s="12" t="s">
+      <c r="E365" s="12" t="s">
         <v>249</v>
-      </c>
-      <c r="E365" s="12" t="s">
-        <v>250</v>
       </c>
       <c r="G365" s="12" t="s">
         <v>4</v>
@@ -11809,7 +11861,7 @@
     </row>
     <row r="366" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B366" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G366" s="12" t="s">
         <v>4</v>
@@ -11827,7 +11879,7 @@
     <row r="367" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A367" s="10"/>
       <c r="B367" s="10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C367" s="10"/>
       <c r="D367" s="10"/>
@@ -11854,7 +11906,7 @@
     </row>
     <row r="368" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B368" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G368" s="12" t="s">
         <v>4</v>
@@ -11872,7 +11924,7 @@
     <row r="369" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A369" s="10"/>
       <c r="B369" s="10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C369" s="10"/>
       <c r="D369" s="10"/>
@@ -11884,7 +11936,7 @@
       <c r="H369" s="10"/>
       <c r="I369" s="10"/>
       <c r="J369" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K369" s="10"/>
       <c r="L369" s="10"/>
@@ -11902,7 +11954,7 @@
     <row r="370" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A370" s="10"/>
       <c r="B370" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C370" s="10"/>
       <c r="D370" s="10"/>
@@ -11930,7 +11982,7 @@
     <row r="371" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A371" s="10"/>
       <c r="B371" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C371" s="10"/>
       <c r="D371" s="10"/>
@@ -11958,7 +12010,7 @@
     <row r="372" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A372" s="10"/>
       <c r="B372" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C372" s="10"/>
       <c r="D372" s="10"/>
@@ -11986,7 +12038,7 @@
     <row r="373" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A373" s="10"/>
       <c r="B373" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C373" s="10"/>
       <c r="D373" s="10"/>
@@ -12014,7 +12066,7 @@
     <row r="374" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A374" s="10"/>
       <c r="B374" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C374" s="10"/>
       <c r="D374" s="10"/>
@@ -12042,7 +12094,7 @@
     <row r="375" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A375" s="10"/>
       <c r="B375" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C375" s="10"/>
       <c r="D375" s="10"/>
@@ -12070,7 +12122,7 @@
     <row r="376" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A376" s="10"/>
       <c r="B376" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C376" s="10"/>
       <c r="D376" s="10"/>
@@ -12098,7 +12150,7 @@
     <row r="377" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A377" s="10"/>
       <c r="B377" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C377" s="10"/>
       <c r="D377" s="10"/>
@@ -12126,7 +12178,7 @@
     <row r="378" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A378" s="10"/>
       <c r="B378" s="10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C378" s="10"/>
       <c r="D378" s="10"/>
@@ -12154,7 +12206,7 @@
     <row r="379" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A379" s="10"/>
       <c r="B379" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C379" s="10"/>
       <c r="D379" s="10"/>
@@ -12182,7 +12234,7 @@
     <row r="380" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A380" s="10"/>
       <c r="B380" s="10" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C380" s="10"/>
       <c r="D380" s="10"/>
@@ -12210,7 +12262,7 @@
     <row r="381" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A381" s="10"/>
       <c r="B381" s="10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C381" s="10"/>
       <c r="D381" s="10"/>
@@ -12237,13 +12289,13 @@
     </row>
     <row r="382" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B382" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G382" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J382" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K382" s="13"/>
       <c r="O382" s="12">
@@ -12257,7 +12309,7 @@
     </row>
     <row r="383" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B383" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G383" s="12" t="s">
         <v>4</v>
@@ -12274,7 +12326,7 @@
     </row>
     <row r="384" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B384" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G384" s="12" t="s">
         <v>4</v>
@@ -12291,7 +12343,7 @@
     </row>
     <row r="385" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B385" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G385" s="12" t="s">
         <v>4</v>
@@ -12308,7 +12360,7 @@
     </row>
     <row r="386" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B386" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G386" s="12" t="s">
         <v>4</v>
@@ -12325,7 +12377,7 @@
     </row>
     <row r="387" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B387" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G387" s="12" t="s">
         <v>4</v>
@@ -12343,7 +12395,7 @@
     <row r="388" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A388" s="10"/>
       <c r="B388" s="10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C388" s="10"/>
       <c r="D388" s="10"/>
@@ -12371,7 +12423,7 @@
     <row r="389" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A389" s="10"/>
       <c r="B389" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C389" s="10"/>
       <c r="D389" s="10"/>
@@ -12399,7 +12451,7 @@
     <row r="390" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A390" s="10"/>
       <c r="B390" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C390" s="10"/>
       <c r="D390" s="10"/>
@@ -12427,7 +12479,7 @@
     <row r="391" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A391" s="10"/>
       <c r="B391" s="10" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C391" s="10"/>
       <c r="D391" s="10"/>
@@ -12454,7 +12506,7 @@
     </row>
     <row r="392" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B392" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G392" s="12" t="s">
         <v>4</v>
@@ -12471,7 +12523,7 @@
     </row>
     <row r="393" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B393" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G393" s="12" t="s">
         <v>4</v>
@@ -12489,10 +12541,10 @@
     <row r="394" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A394" s="10"/>
       <c r="B394" s="10" t="s">
+        <v>562</v>
+      </c>
+      <c r="C394" s="10" t="s">
         <v>563</v>
-      </c>
-      <c r="C394" s="10" t="s">
-        <v>564</v>
       </c>
       <c r="D394" s="10"/>
       <c r="E394" s="10" t="s">
@@ -12523,7 +12575,7 @@
     <row r="395" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A395" s="10"/>
       <c r="B395" s="10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C395" s="10"/>
       <c r="D395" s="10"/>
@@ -12550,7 +12602,7 @@
     </row>
     <row r="396" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B396" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G396" s="12" t="s">
         <v>4</v>
@@ -12567,7 +12619,7 @@
     </row>
     <row r="397" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B397" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G397" s="12" t="s">
         <v>4</v>
@@ -12845,7 +12897,7 @@
         <v>86</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -12867,7 +12919,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>88</v>
@@ -12917,7 +12969,7 @@
         <v>98</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -12950,7 +13002,7 @@
         <v>103</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -12961,7 +13013,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -12991,10 +13043,10 @@
         <v>114</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -13002,10 +13054,10 @@
         <v>115</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -13013,10 +13065,10 @@
         <v>116</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -13024,21 +13076,21 @@
         <v>117</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -13116,7 +13168,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Results of discussion 16-4
</commit_message>
<xml_diff>
--- a/inputs/AddictO_HUman_behaviour_Defs.xlsx
+++ b/inputs/AddictO_HUman_behaviour_Defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5732E45-81D5-4C3F-86FE-CB90DC2CE02D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7603793D-35AF-4AA3-A1BF-5816199D70F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="633">
   <si>
     <t>ID</t>
   </si>
@@ -1919,6 +1919,15 @@
   </si>
   <si>
     <t>Abstinence only has any meaning when specifying what the behaviour is that the person is not doing.</t>
+  </si>
+  <si>
+    <t>Substance use that involves using a combustible product to inhale smoke.</t>
+  </si>
+  <si>
+    <t>Tobacco smoking</t>
+  </si>
+  <si>
+    <t>Smoking in which the combustion product is a tobacco containing product.</t>
   </si>
 </sst>
 </file>
@@ -2443,11 +2452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T422"/>
+  <dimension ref="A1:T423"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B363" sqref="B363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10885,6 +10894,9 @@
       <c r="B324" s="12" t="s">
         <v>223</v>
       </c>
+      <c r="C324" s="12" t="s">
+        <v>630</v>
+      </c>
       <c r="G324" s="12" t="s">
         <v>4</v>
       </c>
@@ -11793,35 +11805,29 @@
       <c r="S362" s="13"/>
       <c r="T362" s="10"/>
     </row>
-    <row r="363" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B363" s="12" t="s">
-        <v>243</v>
+        <v>631</v>
       </c>
       <c r="C363" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="E363" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="F363" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G363" s="12" t="s">
-        <v>4</v>
+        <v>632</v>
       </c>
       <c r="K363" s="13"/>
-      <c r="O363" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q363" s="12" t="s">
-        <v>123</v>
-      </c>
       <c r="S363" s="13"/>
       <c r="T363" s="10"/>
     </row>
-    <row r="364" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B364" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="C364" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E364" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F364" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="G364" s="12" t="s">
         <v>4</v>
@@ -11838,13 +11844,7 @@
     </row>
     <row r="365" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B365" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="C365" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="E365" s="12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G365" s="12" t="s">
         <v>4</v>
@@ -11861,7 +11861,13 @@
     </row>
     <row r="366" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B366" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
+      </c>
+      <c r="C366" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="E366" s="12" t="s">
+        <v>249</v>
       </c>
       <c r="G366" s="12" t="s">
         <v>4</v>
@@ -11877,84 +11883,71 @@
       <c r="T366" s="10"/>
     </row>
     <row r="367" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A367" s="10"/>
-      <c r="B367" s="10" t="s">
+      <c r="B367" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="G367" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K367" s="13"/>
+      <c r="O367" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q367" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S367" s="13"/>
+      <c r="T367" s="10"/>
+    </row>
+    <row r="368" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A368" s="10"/>
+      <c r="B368" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="C367" s="10"/>
-      <c r="D367" s="10"/>
-      <c r="E367" s="10"/>
-      <c r="F367" s="10"/>
-      <c r="G367" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H367" s="10"/>
-      <c r="I367" s="10"/>
-      <c r="J367" s="10"/>
-      <c r="K367" s="10"/>
-      <c r="L367" s="10"/>
-      <c r="M367" s="10"/>
-      <c r="N367" s="10"/>
-      <c r="O367" s="10"/>
-      <c r="P367" s="10"/>
-      <c r="Q367" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R367" s="10"/>
-      <c r="S367" s="10"/>
-      <c r="T367" s="10"/>
-    </row>
-    <row r="368" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B368" s="12" t="s">
+      <c r="C368" s="10"/>
+      <c r="D368" s="10"/>
+      <c r="E368" s="10"/>
+      <c r="F368" s="10"/>
+      <c r="G368" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H368" s="10"/>
+      <c r="I368" s="10"/>
+      <c r="J368" s="10"/>
+      <c r="K368" s="10"/>
+      <c r="L368" s="10"/>
+      <c r="M368" s="10"/>
+      <c r="N368" s="10"/>
+      <c r="O368" s="10"/>
+      <c r="P368" s="10"/>
+      <c r="Q368" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="R368" s="10"/>
+      <c r="S368" s="10"/>
+      <c r="T368" s="10"/>
+    </row>
+    <row r="369" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B369" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="G368" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K368" s="13"/>
-      <c r="O368" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q368" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="S368" s="13"/>
-      <c r="T368" s="10"/>
-    </row>
-    <row r="369" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A369" s="10"/>
-      <c r="B369" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="C369" s="10"/>
-      <c r="D369" s="10"/>
-      <c r="E369" s="10"/>
-      <c r="F369" s="10"/>
-      <c r="G369" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H369" s="10"/>
-      <c r="I369" s="10"/>
-      <c r="J369" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="K369" s="10"/>
-      <c r="L369" s="10"/>
-      <c r="M369" s="10"/>
-      <c r="N369" s="10"/>
-      <c r="O369" s="10"/>
-      <c r="P369" s="10"/>
-      <c r="Q369" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R369" s="10"/>
-      <c r="S369" s="10"/>
+      <c r="G369" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K369" s="13"/>
+      <c r="O369" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q369" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S369" s="13"/>
       <c r="T369" s="10"/>
     </row>
-    <row r="370" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A370" s="10"/>
       <c r="B370" s="10" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C370" s="10"/>
       <c r="D370" s="10"/>
@@ -11965,7 +11958,9 @@
       </c>
       <c r="H370" s="10"/>
       <c r="I370" s="10"/>
-      <c r="J370" s="10"/>
+      <c r="J370" s="10" t="s">
+        <v>545</v>
+      </c>
       <c r="K370" s="10"/>
       <c r="L370" s="10"/>
       <c r="M370" s="10"/>
@@ -11979,10 +11974,10 @@
       <c r="S370" s="10"/>
       <c r="T370" s="10"/>
     </row>
-    <row r="371" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A371" s="10"/>
       <c r="B371" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C371" s="10"/>
       <c r="D371" s="10"/>
@@ -12007,10 +12002,10 @@
       <c r="S371" s="10"/>
       <c r="T371" s="10"/>
     </row>
-    <row r="372" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A372" s="10"/>
       <c r="B372" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C372" s="10"/>
       <c r="D372" s="10"/>
@@ -12035,10 +12030,10 @@
       <c r="S372" s="10"/>
       <c r="T372" s="10"/>
     </row>
-    <row r="373" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A373" s="10"/>
       <c r="B373" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C373" s="10"/>
       <c r="D373" s="10"/>
@@ -12063,10 +12058,10 @@
       <c r="S373" s="10"/>
       <c r="T373" s="10"/>
     </row>
-    <row r="374" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A374" s="10"/>
       <c r="B374" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C374" s="10"/>
       <c r="D374" s="10"/>
@@ -12094,7 +12089,7 @@
     <row r="375" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A375" s="10"/>
       <c r="B375" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C375" s="10"/>
       <c r="D375" s="10"/>
@@ -12122,7 +12117,7 @@
     <row r="376" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A376" s="10"/>
       <c r="B376" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C376" s="10"/>
       <c r="D376" s="10"/>
@@ -12147,10 +12142,10 @@
       <c r="S376" s="10"/>
       <c r="T376" s="10"/>
     </row>
-    <row r="377" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A377" s="10"/>
       <c r="B377" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C377" s="10"/>
       <c r="D377" s="10"/>
@@ -12178,7 +12173,7 @@
     <row r="378" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A378" s="10"/>
       <c r="B378" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C378" s="10"/>
       <c r="D378" s="10"/>
@@ -12203,10 +12198,10 @@
       <c r="S378" s="10"/>
       <c r="T378" s="10"/>
     </row>
-    <row r="379" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:20" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A379" s="10"/>
       <c r="B379" s="10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C379" s="10"/>
       <c r="D379" s="10"/>
@@ -12234,7 +12229,7 @@
     <row r="380" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A380" s="10"/>
       <c r="B380" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C380" s="10"/>
       <c r="D380" s="10"/>
@@ -12262,7 +12257,7 @@
     <row r="381" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A381" s="10"/>
       <c r="B381" s="10" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C381" s="10"/>
       <c r="D381" s="10"/>
@@ -12288,31 +12283,42 @@
       <c r="T381" s="10"/>
     </row>
     <row r="382" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B382" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="G382" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J382" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="K382" s="13"/>
-      <c r="O382" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q382" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="S382" s="13"/>
+      <c r="A382" s="10"/>
+      <c r="B382" s="10" t="s">
+        <v>557</v>
+      </c>
+      <c r="C382" s="10"/>
+      <c r="D382" s="10"/>
+      <c r="E382" s="10"/>
+      <c r="F382" s="10"/>
+      <c r="G382" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H382" s="10"/>
+      <c r="I382" s="10"/>
+      <c r="J382" s="10"/>
+      <c r="K382" s="10"/>
+      <c r="L382" s="10"/>
+      <c r="M382" s="10"/>
+      <c r="N382" s="10"/>
+      <c r="O382" s="10"/>
+      <c r="P382" s="10"/>
+      <c r="Q382" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="R382" s="10"/>
+      <c r="S382" s="10"/>
       <c r="T382" s="10"/>
     </row>
     <row r="383" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B383" s="12" t="s">
-        <v>253</v>
+        <v>136</v>
       </c>
       <c r="G383" s="12" t="s">
         <v>4</v>
+      </c>
+      <c r="J383" s="12" t="s">
+        <v>252</v>
       </c>
       <c r="K383" s="13"/>
       <c r="O383" s="12">
@@ -12326,7 +12332,7 @@
     </row>
     <row r="384" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B384" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G384" s="12" t="s">
         <v>4</v>
@@ -12343,7 +12349,7 @@
     </row>
     <row r="385" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B385" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G385" s="12" t="s">
         <v>4</v>
@@ -12360,7 +12366,7 @@
     </row>
     <row r="386" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B386" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G386" s="12" t="s">
         <v>4</v>
@@ -12377,7 +12383,7 @@
     </row>
     <row r="387" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B387" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G387" s="12" t="s">
         <v>4</v>
@@ -12393,37 +12399,26 @@
       <c r="T387" s="10"/>
     </row>
     <row r="388" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A388" s="10"/>
-      <c r="B388" s="10" t="s">
-        <v>558</v>
-      </c>
-      <c r="C388" s="10"/>
-      <c r="D388" s="10"/>
-      <c r="E388" s="10"/>
-      <c r="F388" s="10"/>
-      <c r="G388" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H388" s="10"/>
-      <c r="I388" s="10"/>
-      <c r="J388" s="10"/>
-      <c r="K388" s="10"/>
-      <c r="L388" s="10"/>
-      <c r="M388" s="10"/>
-      <c r="N388" s="10"/>
-      <c r="O388" s="10"/>
-      <c r="P388" s="10"/>
-      <c r="Q388" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R388" s="10"/>
-      <c r="S388" s="10"/>
+      <c r="B388" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="G388" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K388" s="13"/>
+      <c r="O388" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q388" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S388" s="13"/>
       <c r="T388" s="10"/>
     </row>
     <row r="389" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A389" s="10"/>
       <c r="B389" s="10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C389" s="10"/>
       <c r="D389" s="10"/>
@@ -12451,7 +12446,7 @@
     <row r="390" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A390" s="10"/>
       <c r="B390" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C390" s="10"/>
       <c r="D390" s="10"/>
@@ -12479,7 +12474,7 @@
     <row r="391" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A391" s="10"/>
       <c r="B391" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C391" s="10"/>
       <c r="D391" s="10"/>
@@ -12505,25 +12500,36 @@
       <c r="T391" s="10"/>
     </row>
     <row r="392" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B392" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="G392" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K392" s="13"/>
-      <c r="O392" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q392" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="S392" s="13"/>
+      <c r="A392" s="10"/>
+      <c r="B392" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="C392" s="10"/>
+      <c r="D392" s="10"/>
+      <c r="E392" s="10"/>
+      <c r="F392" s="10"/>
+      <c r="G392" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H392" s="10"/>
+      <c r="I392" s="10"/>
+      <c r="J392" s="10"/>
+      <c r="K392" s="10"/>
+      <c r="L392" s="10"/>
+      <c r="M392" s="10"/>
+      <c r="N392" s="10"/>
+      <c r="O392" s="10"/>
+      <c r="P392" s="10"/>
+      <c r="Q392" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="R392" s="10"/>
+      <c r="S392" s="10"/>
       <c r="T392" s="10"/>
     </row>
     <row r="393" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B393" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G393" s="12" t="s">
         <v>4</v>
@@ -12539,48 +12545,37 @@
       <c r="T393" s="10"/>
     </row>
     <row r="394" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A394" s="10"/>
-      <c r="B394" s="10" t="s">
-        <v>562</v>
-      </c>
-      <c r="C394" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="D394" s="10"/>
-      <c r="E394" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F394" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G394" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H394" s="10"/>
-      <c r="I394" s="10"/>
-      <c r="J394" s="10"/>
-      <c r="K394" s="10"/>
-      <c r="L394" s="10"/>
-      <c r="M394" s="10"/>
-      <c r="N394" s="10"/>
-      <c r="O394" s="10"/>
-      <c r="P394" s="10"/>
-      <c r="Q394" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R394" s="10"/>
-      <c r="S394" s="10"/>
+      <c r="B394" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="G394" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K394" s="13"/>
+      <c r="O394" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q394" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S394" s="13"/>
       <c r="T394" s="10"/>
     </row>
     <row r="395" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A395" s="10"/>
       <c r="B395" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="C395" s="10"/>
+        <v>562</v>
+      </c>
+      <c r="C395" s="10" t="s">
+        <v>563</v>
+      </c>
       <c r="D395" s="10"/>
-      <c r="E395" s="10"/>
-      <c r="F395" s="10"/>
+      <c r="E395" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F395" s="10" t="s">
+        <v>127</v>
+      </c>
       <c r="G395" s="10" t="s">
         <v>4</v>
       </c>
@@ -12601,25 +12596,36 @@
       <c r="T395" s="10"/>
     </row>
     <row r="396" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B396" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="G396" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K396" s="13"/>
-      <c r="O396" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q396" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="S396" s="13"/>
+      <c r="A396" s="10"/>
+      <c r="B396" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="C396" s="10"/>
+      <c r="D396" s="10"/>
+      <c r="E396" s="10"/>
+      <c r="F396" s="10"/>
+      <c r="G396" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H396" s="10"/>
+      <c r="I396" s="10"/>
+      <c r="J396" s="10"/>
+      <c r="K396" s="10"/>
+      <c r="L396" s="10"/>
+      <c r="M396" s="10"/>
+      <c r="N396" s="10"/>
+      <c r="O396" s="10"/>
+      <c r="P396" s="10"/>
+      <c r="Q396" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="R396" s="10"/>
+      <c r="S396" s="10"/>
       <c r="T396" s="10"/>
     </row>
     <row r="397" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B397" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G397" s="12" t="s">
         <v>4</v>
@@ -12634,87 +12640,86 @@
       <c r="S397" s="13"/>
       <c r="T397" s="10"/>
     </row>
-    <row r="398" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B398" s="13"/>
-      <c r="Q398" s="10" t="s">
-        <v>123</v>
-      </c>
+    <row r="398" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B398" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="G398" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K398" s="13"/>
+      <c r="O398" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q398" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="S398" s="13"/>
+      <c r="T398" s="10"/>
     </row>
     <row r="399" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B399" s="13"/>
-      <c r="G399" s="11"/>
-      <c r="H399" s="11"/>
-      <c r="I399" s="13"/>
-      <c r="J399" s="11"/>
-      <c r="K399" s="11"/>
-      <c r="L399" s="11"/>
-      <c r="M399" s="11">
-        <v>1</v>
-      </c>
-      <c r="N399" s="11"/>
-      <c r="O399" s="11"/>
-      <c r="P399" s="11"/>
-      <c r="Q399" s="11"/>
+      <c r="Q399" s="10" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="400" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B400" s="13"/>
-      <c r="Q400" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="401" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G400" s="11"/>
+      <c r="H400" s="11"/>
+      <c r="I400" s="13"/>
+      <c r="J400" s="11"/>
+      <c r="K400" s="11"/>
+      <c r="L400" s="11"/>
+      <c r="M400" s="11">
+        <v>1</v>
+      </c>
+      <c r="N400" s="11"/>
+      <c r="O400" s="11"/>
+      <c r="P400" s="11"/>
+      <c r="Q400" s="11"/>
+    </row>
+    <row r="401" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B401" s="13"/>
       <c r="Q401" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="402" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B402" s="13"/>
       <c r="Q402" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="403" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B403" s="13"/>
-      <c r="E403" s="11"/>
-      <c r="F403" s="11"/>
-      <c r="G403" s="11"/>
-      <c r="H403" s="11"/>
-      <c r="I403" s="11"/>
-      <c r="J403" s="11"/>
-      <c r="K403" s="11"/>
-      <c r="L403" s="11"/>
-      <c r="M403" s="11"/>
-      <c r="N403" s="11"/>
-      <c r="O403" s="11"/>
-      <c r="P403" s="11"/>
-      <c r="Q403" s="11"/>
-    </row>
-    <row r="404" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q403" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="404" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B404" s="13"/>
-      <c r="Q404" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="405" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E404" s="11"/>
+      <c r="F404" s="11"/>
+      <c r="G404" s="11"/>
+      <c r="H404" s="11"/>
+      <c r="I404" s="11"/>
+      <c r="J404" s="11"/>
+      <c r="K404" s="11"/>
+      <c r="L404" s="11"/>
+      <c r="M404" s="11"/>
+      <c r="N404" s="11"/>
+      <c r="O404" s="11"/>
+      <c r="P404" s="11"/>
+      <c r="Q404" s="11"/>
+    </row>
+    <row r="405" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B405" s="13"/>
-      <c r="C405" s="11"/>
-      <c r="D405" s="21"/>
-      <c r="E405" s="11"/>
-      <c r="F405" s="11"/>
-      <c r="G405" s="11"/>
-      <c r="H405" s="11"/>
-      <c r="I405" s="11"/>
-      <c r="J405" s="11"/>
-      <c r="K405" s="11"/>
-      <c r="L405" s="11"/>
-      <c r="M405" s="11"/>
-      <c r="N405" s="11"/>
-      <c r="O405" s="11"/>
-      <c r="P405" s="11"/>
-      <c r="Q405" s="11"/>
-    </row>
-    <row r="406" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q405" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="406" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B406" s="13"/>
       <c r="C406" s="11"/>
       <c r="D406" s="21"/>
@@ -12732,60 +12737,60 @@
       <c r="P406" s="11"/>
       <c r="Q406" s="11"/>
     </row>
-    <row r="407" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="407" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B407" s="13"/>
-      <c r="R407" s="11"/>
-    </row>
-    <row r="408" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C407" s="11"/>
+      <c r="D407" s="21"/>
+      <c r="E407" s="11"/>
+      <c r="F407" s="11"/>
+      <c r="G407" s="11"/>
+      <c r="H407" s="11"/>
+      <c r="I407" s="11"/>
+      <c r="J407" s="11"/>
+      <c r="K407" s="11"/>
+      <c r="L407" s="11"/>
+      <c r="M407" s="11"/>
+      <c r="N407" s="11"/>
+      <c r="O407" s="11"/>
+      <c r="P407" s="11"/>
+      <c r="Q407" s="11"/>
+    </row>
+    <row r="408" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B408" s="13"/>
-    </row>
-    <row r="409" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="R408" s="11"/>
+    </row>
+    <row r="409" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B409" s="13"/>
     </row>
-    <row r="410" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="410" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B410" s="13"/>
     </row>
-    <row r="411" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="411" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B411" s="13"/>
     </row>
-    <row r="412" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="412" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B412" s="13"/>
     </row>
-    <row r="413" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="413" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B413" s="13"/>
     </row>
-    <row r="414" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="414" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B414" s="13"/>
     </row>
-    <row r="415" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="415" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B415" s="13"/>
     </row>
-    <row r="416" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A416" s="13"/>
+    <row r="416" spans="2:18" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B416" s="13"/>
-      <c r="S416" s="11"/>
     </row>
     <row r="417" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A417" s="13"/>
       <c r="B417" s="13"/>
-      <c r="R417" s="11"/>
+      <c r="S417" s="11"/>
     </row>
     <row r="418" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B418" s="13"/>
-      <c r="C418" s="11"/>
-      <c r="D418" s="21"/>
-      <c r="E418" s="11"/>
-      <c r="F418" s="11"/>
-      <c r="G418" s="11"/>
-      <c r="H418" s="11"/>
-      <c r="I418" s="11"/>
-      <c r="J418" s="11"/>
-      <c r="K418" s="11"/>
-      <c r="L418" s="11"/>
-      <c r="M418" s="11"/>
-      <c r="N418" s="11"/>
-      <c r="O418" s="11"/>
-      <c r="P418" s="11"/>
-      <c r="Q418" s="11"/>
+      <c r="R418" s="11"/>
     </row>
     <row r="419" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B419" s="13"/>
@@ -12804,10 +12809,8 @@
       <c r="O419" s="11"/>
       <c r="P419" s="11"/>
       <c r="Q419" s="11"/>
-      <c r="R419" s="11"/>
     </row>
     <row r="420" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A420" s="11"/>
       <c r="B420" s="13"/>
       <c r="C420" s="11"/>
       <c r="D420" s="21"/>
@@ -12825,9 +12828,9 @@
       <c r="P420" s="11"/>
       <c r="Q420" s="11"/>
       <c r="R420" s="11"/>
-      <c r="S420" s="11"/>
     </row>
     <row r="421" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A421" s="11"/>
       <c r="B421" s="13"/>
       <c r="C421" s="11"/>
       <c r="D421" s="21"/>
@@ -12845,13 +12848,33 @@
       <c r="P421" s="11"/>
       <c r="Q421" s="11"/>
       <c r="R421" s="11"/>
-    </row>
-    <row r="422" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S421" s="11"/>
+    </row>
+    <row r="422" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B422" s="13"/>
+      <c r="C422" s="11"/>
+      <c r="D422" s="21"/>
+      <c r="E422" s="11"/>
+      <c r="F422" s="11"/>
+      <c r="G422" s="11"/>
+      <c r="H422" s="11"/>
+      <c r="I422" s="11"/>
+      <c r="J422" s="11"/>
+      <c r="K422" s="11"/>
+      <c r="L422" s="11"/>
+      <c r="M422" s="11"/>
+      <c r="N422" s="11"/>
+      <c r="O422" s="11"/>
+      <c r="P422" s="11"/>
+      <c r="Q422" s="11"/>
+      <c r="R422" s="11"/>
+    </row>
+    <row r="423" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B423" s="13"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T420">
-    <sortCondition ref="B2:B420"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T421">
+    <sortCondition ref="B2:B421"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates based on discussion
</commit_message>
<xml_diff>
--- a/inputs/AddictO_HUman_behaviour_Defs.xlsx
+++ b/inputs/AddictO_HUman_behaviour_Defs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeed\Documents\GitHub\addiction-ontology\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharoncox/Documents/GitHub/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7038E1FC-4EB6-EF4B-BFB3-69DC157609DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Upper level diagram" sheetId="6" r:id="rId4"/>
     <sheet name="Links" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1968,7 +1969,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2198,7 +2199,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2495,39 +2496,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T427"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
+      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B263" sqref="B263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="11" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="64.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="64.5" style="21" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="11" customWidth="1"/>
     <col min="7" max="7" width="16" style="11" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="48.28515625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="11" customWidth="1"/>
-    <col min="12" max="12" width="44.140625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="11"/>
-    <col min="14" max="14" width="18.42578125" style="11" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="11"/>
-    <col min="17" max="17" width="13.42578125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="37.140625" style="11" customWidth="1"/>
-    <col min="19" max="19" width="48.7109375" style="11" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" style="11" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="11"/>
+    <col min="8" max="8" width="35.5" style="11" customWidth="1"/>
+    <col min="9" max="9" width="48.33203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="11" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="44.1640625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="11"/>
+    <col min="14" max="14" width="18.5" style="11" customWidth="1"/>
+    <col min="15" max="16" width="9.1640625" style="11"/>
+    <col min="17" max="17" width="13.5" style="11" customWidth="1"/>
+    <col min="18" max="18" width="37.1640625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="48.6640625" style="11" customWidth="1"/>
+    <col min="20" max="20" width="24.6640625" style="11" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2586,7 +2587,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>118</v>
       </c>
@@ -2615,7 +2616,7 @@
       <c r="S2" s="13"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>124</v>
       </c>
@@ -2641,7 +2642,7 @@
       <c r="S3" s="13"/>
       <c r="T3" s="11"/>
     </row>
-    <row r="4" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>128</v>
       </c>
@@ -2667,7 +2668,7 @@
       <c r="S4" s="13"/>
       <c r="T4" s="11"/>
     </row>
-    <row r="5" spans="1:20" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>130</v>
       </c>
@@ -2693,7 +2694,7 @@
       <c r="S5" s="13"/>
       <c r="T5" s="11"/>
     </row>
-    <row r="6" spans="1:20" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="25" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" s="25" t="s">
         <v>132</v>
       </c>
@@ -2721,7 +2722,7 @@
       <c r="S6" s="28"/>
       <c r="T6" s="26"/>
     </row>
-    <row r="7" spans="1:20" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
         <v>262</v>
@@ -2755,7 +2756,7 @@
       <c r="S7" s="10"/>
       <c r="T7" s="11"/>
     </row>
-    <row r="8" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>134</v>
       </c>
@@ -2781,7 +2782,7 @@
       <c r="S8" s="13"/>
       <c r="T8" s="11"/>
     </row>
-    <row r="9" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
         <v>264</v>
@@ -2815,7 +2816,7 @@
       <c r="S9" s="10"/>
       <c r="T9" s="11"/>
     </row>
-    <row r="10" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>135</v>
       </c>
@@ -2841,7 +2842,7 @@
       <c r="S10" s="13"/>
       <c r="T10" s="11"/>
     </row>
-    <row r="11" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>137</v>
       </c>
@@ -2870,7 +2871,7 @@
       <c r="S11" s="13"/>
       <c r="T11" s="11"/>
     </row>
-    <row r="12" spans="1:20" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="17" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="16" t="s">
         <v>605</v>
@@ -2912,7 +2913,7 @@
       <c r="S12" s="16"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
         <v>268</v>
@@ -2950,7 +2951,7 @@
       <c r="S13" s="10"/>
       <c r="T13" s="11"/>
     </row>
-    <row r="14" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
         <v>269</v>
@@ -2988,7 +2989,7 @@
       <c r="S14" s="10"/>
       <c r="T14" s="11"/>
     </row>
-    <row r="15" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
         <v>270</v>
@@ -3021,7 +3022,7 @@
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
     </row>
-    <row r="16" spans="1:20" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
         <v>271</v>
@@ -3054,7 +3055,7 @@
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
     </row>
-    <row r="17" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
         <v>273</v>
@@ -3085,7 +3086,7 @@
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
     </row>
-    <row r="18" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10" t="s">
         <v>274</v>
@@ -3116,7 +3117,7 @@
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
     </row>
-    <row r="19" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
         <v>275</v>
@@ -3147,7 +3148,7 @@
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
     </row>
-    <row r="20" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>276</v>
@@ -3178,7 +3179,7 @@
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
     </row>
-    <row r="21" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="10" t="s">
         <v>277</v>
@@ -3209,7 +3210,7 @@
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
     </row>
-    <row r="22" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="s">
         <v>278</v>
@@ -3240,7 +3241,7 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
     </row>
-    <row r="23" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="s">
         <v>279</v>
@@ -3267,7 +3268,7 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" s="16" t="s">
         <v>272</v>
@@ -3302,7 +3303,7 @@
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
     </row>
-    <row r="25" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
         <v>283</v>
@@ -3331,7 +3332,7 @@
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
     </row>
-    <row r="26" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
         <v>284</v>
@@ -3358,7 +3359,7 @@
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
     </row>
-    <row r="27" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
         <v>285</v>
@@ -3385,7 +3386,7 @@
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
     </row>
-    <row r="28" spans="1:19" s="12" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="12" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
         <v>286</v>
@@ -3416,7 +3417,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
         <v>288</v>
@@ -3443,7 +3444,7 @@
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
     </row>
-    <row r="30" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="10" t="s">
         <v>289</v>
@@ -3470,7 +3471,7 @@
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
     </row>
-    <row r="31" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="10" t="s">
         <v>290</v>
@@ -3497,7 +3498,7 @@
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
     </row>
-    <row r="32" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
         <v>291</v>
@@ -3524,7 +3525,7 @@
       <c r="R32" s="10"/>
       <c r="S32" s="10"/>
     </row>
-    <row r="33" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>292</v>
@@ -3551,7 +3552,7 @@
       <c r="R33" s="10"/>
       <c r="S33" s="10"/>
     </row>
-    <row r="34" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="10" t="s">
         <v>293</v>
@@ -3578,7 +3579,7 @@
       <c r="R34" s="10"/>
       <c r="S34" s="10"/>
     </row>
-    <row r="35" spans="1:19" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="17" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>593</v>
       </c>
@@ -3613,7 +3614,7 @@
       <c r="R35" s="16"/>
       <c r="S35" s="16"/>
     </row>
-    <row r="36" spans="1:19" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
         <v>595</v>
       </c>
@@ -3635,7 +3636,7 @@
       </c>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:19" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
         <v>597</v>
       </c>
@@ -3657,7 +3658,7 @@
       </c>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="1:19" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
         <v>600</v>
       </c>
@@ -3679,7 +3680,7 @@
       </c>
       <c r="N38" s="18"/>
     </row>
-    <row r="39" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>295</v>
@@ -3708,7 +3709,7 @@
       <c r="R39" s="10"/>
       <c r="S39" s="10"/>
     </row>
-    <row r="40" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>139</v>
@@ -3739,7 +3740,7 @@
       <c r="R40" s="10"/>
       <c r="S40" s="10"/>
     </row>
-    <row r="41" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
         <v>299</v>
@@ -3768,7 +3769,7 @@
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
     </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="10" t="s">
         <v>282</v>
@@ -3799,7 +3800,7 @@
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
     </row>
-    <row r="43" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
         <v>301</v>
@@ -3826,7 +3827,7 @@
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
     </row>
-    <row r="44" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="10" t="s">
         <v>539</v>
@@ -3859,7 +3860,7 @@
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
     </row>
-    <row r="45" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
       <c r="B45" s="10" t="s">
         <v>249</v>
@@ -3892,7 +3893,7 @@
       <c r="R45" s="10"/>
       <c r="S45" s="10"/>
     </row>
-    <row r="46" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
       <c r="B46" s="10" t="s">
         <v>302</v>
@@ -3919,7 +3920,7 @@
       <c r="R46" s="10"/>
       <c r="S46" s="10"/>
     </row>
-    <row r="47" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
       <c r="B47" s="10" t="s">
         <v>303</v>
@@ -3946,7 +3947,7 @@
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
     </row>
-    <row r="48" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="10"/>
       <c r="B48" s="10" t="s">
         <v>304</v>
@@ -3973,7 +3974,7 @@
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
     </row>
-    <row r="49" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
       <c r="B49" s="10" t="s">
         <v>305</v>
@@ -4000,7 +4001,7 @@
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
     </row>
-    <row r="50" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="10"/>
       <c r="B50" s="10" t="s">
         <v>306</v>
@@ -4027,7 +4028,7 @@
       <c r="R50" s="10"/>
       <c r="S50" s="10"/>
     </row>
-    <row r="51" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
       <c r="B51" s="10" t="s">
         <v>307</v>
@@ -4054,7 +4055,7 @@
       <c r="R51" s="10"/>
       <c r="S51" s="10"/>
     </row>
-    <row r="52" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
       <c r="B52" s="10" t="s">
         <v>308</v>
@@ -4081,7 +4082,7 @@
       <c r="R52" s="10"/>
       <c r="S52" s="10"/>
     </row>
-    <row r="53" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>309</v>
@@ -4108,7 +4109,7 @@
       <c r="R53" s="10"/>
       <c r="S53" s="10"/>
     </row>
-    <row r="54" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="10"/>
       <c r="B54" s="10" t="s">
         <v>310</v>
@@ -4135,7 +4136,7 @@
       <c r="R54" s="10"/>
       <c r="S54" s="10"/>
     </row>
-    <row r="55" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="10"/>
       <c r="B55" s="10" t="s">
         <v>311</v>
@@ -4162,7 +4163,7 @@
       <c r="R55" s="10"/>
       <c r="S55" s="10"/>
     </row>
-    <row r="56" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="10"/>
       <c r="B56" s="10" t="s">
         <v>312</v>
@@ -4189,7 +4190,7 @@
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
     </row>
-    <row r="57" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="10"/>
       <c r="B57" s="10" t="s">
         <v>313</v>
@@ -4216,7 +4217,7 @@
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
     </row>
-    <row r="58" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="10"/>
       <c r="B58" s="10" t="s">
         <v>314</v>
@@ -4243,7 +4244,7 @@
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
     </row>
-    <row r="59" spans="1:19" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="10"/>
       <c r="B59" s="10" t="s">
         <v>315</v>
@@ -4272,7 +4273,7 @@
       <c r="R59" s="10"/>
       <c r="S59" s="10"/>
     </row>
-    <row r="60" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
       <c r="B60" s="10" t="s">
         <v>317</v>
@@ -4299,7 +4300,7 @@
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
     </row>
-    <row r="61" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="10"/>
       <c r="B61" s="10" t="s">
         <v>318</v>
@@ -4326,7 +4327,7 @@
       <c r="R61" s="10"/>
       <c r="S61" s="10"/>
     </row>
-    <row r="62" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
         <v>319</v>
@@ -4353,7 +4354,7 @@
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
     </row>
-    <row r="63" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
       <c r="B63" s="10" t="s">
         <v>320</v>
@@ -4380,7 +4381,7 @@
       <c r="R63" s="10"/>
       <c r="S63" s="10"/>
     </row>
-    <row r="64" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
       <c r="B64" s="10" t="s">
         <v>321</v>
@@ -4407,7 +4408,7 @@
       <c r="R64" s="10"/>
       <c r="S64" s="10"/>
     </row>
-    <row r="65" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="10"/>
       <c r="B65" s="10" t="s">
         <v>322</v>
@@ -4434,7 +4435,7 @@
       <c r="R65" s="10"/>
       <c r="S65" s="10"/>
     </row>
-    <row r="66" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="10"/>
       <c r="B66" s="10" t="s">
         <v>323</v>
@@ -4461,7 +4462,7 @@
       <c r="R66" s="10"/>
       <c r="S66" s="10"/>
     </row>
-    <row r="67" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="12" t="s">
         <v>140</v>
       </c>
@@ -4477,7 +4478,7 @@
       </c>
       <c r="S67" s="13"/>
     </row>
-    <row r="68" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="12" t="s">
         <v>141</v>
       </c>
@@ -4493,7 +4494,7 @@
       </c>
       <c r="S68" s="13"/>
     </row>
-    <row r="69" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="10"/>
       <c r="B69" s="10" t="s">
         <v>324</v>
@@ -4520,7 +4521,7 @@
       <c r="R69" s="10"/>
       <c r="S69" s="10"/>
     </row>
-    <row r="70" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="12" t="s">
         <v>142</v>
       </c>
@@ -4536,7 +4537,7 @@
       </c>
       <c r="S70" s="13"/>
     </row>
-    <row r="71" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="10"/>
       <c r="B71" s="10" t="s">
         <v>325</v>
@@ -4563,7 +4564,7 @@
       <c r="R71" s="10"/>
       <c r="S71" s="10"/>
     </row>
-    <row r="72" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="10"/>
       <c r="B72" s="10" t="s">
         <v>326</v>
@@ -4590,7 +4591,7 @@
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
     </row>
-    <row r="73" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="10"/>
       <c r="B73" s="10" t="s">
         <v>327</v>
@@ -4617,7 +4618,7 @@
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
     </row>
-    <row r="74" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="10"/>
       <c r="B74" s="10" t="s">
         <v>328</v>
@@ -4644,7 +4645,7 @@
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
     </row>
-    <row r="75" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="11"/>
       <c r="B75" s="11" t="s">
         <v>63</v>
@@ -4675,7 +4676,7 @@
       <c r="R75" s="11"/>
       <c r="S75" s="11"/>
     </row>
-    <row r="76" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="11"/>
       <c r="B76" s="11" t="s">
         <v>64</v>
@@ -4706,7 +4707,7 @@
       <c r="R76" s="11"/>
       <c r="S76" s="11"/>
     </row>
-    <row r="77" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="10"/>
       <c r="B77" s="10" t="s">
         <v>329</v>
@@ -4733,7 +4734,7 @@
       <c r="R77" s="10"/>
       <c r="S77" s="10"/>
     </row>
-    <row r="78" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="12" t="s">
         <v>143</v>
       </c>
@@ -4749,7 +4750,7 @@
       </c>
       <c r="S78" s="13"/>
     </row>
-    <row r="79" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="10"/>
       <c r="B79" s="10" t="s">
         <v>330</v>
@@ -4776,7 +4777,7 @@
       <c r="R79" s="10"/>
       <c r="S79" s="10"/>
     </row>
-    <row r="80" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="10"/>
       <c r="B80" s="10" t="s">
         <v>331</v>
@@ -4803,7 +4804,7 @@
       <c r="R80" s="10"/>
       <c r="S80" s="10"/>
     </row>
-    <row r="81" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="11"/>
       <c r="B81" s="11" t="s">
         <v>111</v>
@@ -4834,7 +4835,7 @@
       <c r="R81" s="11"/>
       <c r="S81" s="11"/>
     </row>
-    <row r="82" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="10"/>
       <c r="B82" s="10" t="s">
         <v>280</v>
@@ -4865,7 +4866,7 @@
       <c r="R82" s="10"/>
       <c r="S82" s="10"/>
     </row>
-    <row r="83" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
       <c r="B83" s="10" t="s">
         <v>334</v>
@@ -4890,7 +4891,7 @@
       <c r="R83" s="10"/>
       <c r="S83" s="10"/>
     </row>
-    <row r="84" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="10"/>
       <c r="B84" s="10" t="s">
         <v>335</v>
@@ -4917,7 +4918,7 @@
       <c r="R84" s="10"/>
       <c r="S84" s="10"/>
     </row>
-    <row r="85" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
       <c r="B85" s="10" t="s">
         <v>336</v>
@@ -4944,7 +4945,7 @@
       <c r="R85" s="10"/>
       <c r="S85" s="10"/>
     </row>
-    <row r="86" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
       <c r="B86" s="10" t="s">
         <v>337</v>
@@ -4971,7 +4972,7 @@
       <c r="R86" s="10"/>
       <c r="S86" s="10"/>
     </row>
-    <row r="87" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="10"/>
       <c r="B87" s="10" t="s">
         <v>144</v>
@@ -4998,7 +4999,7 @@
       <c r="R87" s="10"/>
       <c r="S87" s="10"/>
     </row>
-    <row r="88" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
       <c r="B88" s="10" t="s">
         <v>339</v>
@@ -5023,7 +5024,7 @@
       <c r="R88" s="10"/>
       <c r="S88" s="10"/>
     </row>
-    <row r="89" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
       <c r="B89" s="10" t="s">
         <v>340</v>
@@ -5050,7 +5051,7 @@
       <c r="R89" s="10"/>
       <c r="S89" s="10"/>
     </row>
-    <row r="90" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="10"/>
       <c r="B90" s="12" t="s">
         <v>120</v>
@@ -5075,7 +5076,7 @@
       <c r="R90" s="10"/>
       <c r="S90" s="10"/>
     </row>
-    <row r="91" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B91" s="12" t="s">
         <v>145</v>
       </c>
@@ -5092,7 +5093,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="10" t="s">
         <v>341</v>
       </c>
@@ -5108,7 +5109,7 @@
       </c>
       <c r="S92" s="13"/>
     </row>
-    <row r="93" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="10"/>
       <c r="B93" s="10" t="s">
         <v>342</v>
@@ -5135,7 +5136,7 @@
       <c r="R93" s="10"/>
       <c r="S93" s="10"/>
     </row>
-    <row r="94" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="10"/>
       <c r="B94" s="12" t="s">
         <v>146</v>
@@ -5161,7 +5162,7 @@
       </c>
       <c r="S94" s="10"/>
     </row>
-    <row r="95" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B95" s="12" t="s">
         <v>149</v>
       </c>
@@ -5183,7 +5184,7 @@
       </c>
       <c r="S95" s="13"/>
     </row>
-    <row r="96" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="10"/>
       <c r="B96" s="10" t="s">
         <v>343</v>
@@ -5210,7 +5211,7 @@
       <c r="R96" s="10"/>
       <c r="S96" s="10"/>
     </row>
-    <row r="97" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="10"/>
       <c r="B97" s="10" t="s">
         <v>344</v>
@@ -5237,7 +5238,7 @@
       <c r="R97" s="10"/>
       <c r="S97" s="10"/>
     </row>
-    <row r="98" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="10"/>
       <c r="B98" s="10" t="s">
         <v>345</v>
@@ -5264,7 +5265,7 @@
       <c r="R98" s="10"/>
       <c r="S98" s="10"/>
     </row>
-    <row r="99" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="10"/>
       <c r="B99" s="10" t="s">
         <v>346</v>
@@ -5291,7 +5292,7 @@
       <c r="R99" s="10"/>
       <c r="S99" s="10"/>
     </row>
-    <row r="100" spans="1:19" s="30" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" s="30" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A100" s="31"/>
       <c r="B100" s="29" t="s">
         <v>638</v>
@@ -5330,7 +5331,7 @@
       <c r="R100" s="31"/>
       <c r="S100" s="31"/>
     </row>
-    <row r="101" spans="1:19" s="30" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" s="30" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A101" s="31"/>
       <c r="B101" s="29" t="s">
         <v>642</v>
@@ -5367,7 +5368,7 @@
       <c r="R101" s="31"/>
       <c r="S101" s="31"/>
     </row>
-    <row r="102" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="10"/>
       <c r="B102" s="10" t="s">
         <v>347</v>
@@ -5394,7 +5395,7 @@
       <c r="R102" s="10"/>
       <c r="S102" s="10"/>
     </row>
-    <row r="103" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="10"/>
       <c r="B103" s="10" t="s">
         <v>348</v>
@@ -5421,7 +5422,7 @@
       <c r="R103" s="10"/>
       <c r="S103" s="10"/>
     </row>
-    <row r="104" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="10"/>
       <c r="B104" s="10" t="s">
         <v>349</v>
@@ -5448,7 +5449,7 @@
       <c r="R104" s="10"/>
       <c r="S104" s="10"/>
     </row>
-    <row r="105" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="10"/>
       <c r="B105" s="10" t="s">
         <v>350</v>
@@ -5475,7 +5476,7 @@
       <c r="R105" s="10"/>
       <c r="S105" s="10"/>
     </row>
-    <row r="106" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="10"/>
       <c r="B106" s="10" t="s">
         <v>351</v>
@@ -5502,7 +5503,7 @@
       <c r="R106" s="10"/>
       <c r="S106" s="10"/>
     </row>
-    <row r="107" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="10"/>
       <c r="B107" s="10" t="s">
         <v>352</v>
@@ -5529,7 +5530,7 @@
       <c r="R107" s="10"/>
       <c r="S107" s="10"/>
     </row>
-    <row r="108" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="10"/>
       <c r="B108" s="10" t="s">
         <v>353</v>
@@ -5556,7 +5557,7 @@
       <c r="R108" s="10"/>
       <c r="S108" s="10"/>
     </row>
-    <row r="109" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="10"/>
       <c r="B109" s="10" t="s">
         <v>354</v>
@@ -5585,7 +5586,7 @@
       <c r="R109" s="10"/>
       <c r="S109" s="10"/>
     </row>
-    <row r="110" spans="1:19" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" s="25" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="23"/>
       <c r="B110" s="23" t="s">
         <v>356</v>
@@ -5613,7 +5614,7 @@
       <c r="R110" s="23"/>
       <c r="S110" s="23"/>
     </row>
-    <row r="111" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="10"/>
       <c r="B111" s="10" t="s">
         <v>357</v>
@@ -5642,7 +5643,7 @@
       <c r="R111" s="10"/>
       <c r="S111" s="10"/>
     </row>
-    <row r="112" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="10"/>
       <c r="B112" s="10" t="s">
         <v>359</v>
@@ -5668,7 +5669,7 @@
       <c r="R112" s="10"/>
       <c r="S112" s="10"/>
     </row>
-    <row r="113" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="10"/>
       <c r="B113" s="10" t="s">
         <v>360</v>
@@ -5695,7 +5696,7 @@
       <c r="R113" s="10"/>
       <c r="S113" s="10"/>
     </row>
-    <row r="114" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="10"/>
       <c r="B114" s="10" t="s">
         <v>361</v>
@@ -5723,7 +5724,7 @@
       <c r="S114" s="10"/>
       <c r="T114" s="10"/>
     </row>
-    <row r="115" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="10" t="s">
         <v>362</v>
@@ -5751,7 +5752,7 @@
       <c r="S115" s="10"/>
       <c r="T115" s="10"/>
     </row>
-    <row r="116" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="10"/>
       <c r="B116" s="10" t="s">
         <v>265</v>
@@ -5779,7 +5780,7 @@
       <c r="S116" s="10"/>
       <c r="T116" s="10"/>
     </row>
-    <row r="117" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="10"/>
       <c r="B117" s="10" t="s">
         <v>364</v>
@@ -5811,7 +5812,7 @@
       <c r="S117" s="10"/>
       <c r="T117" s="10"/>
     </row>
-    <row r="118" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="10"/>
       <c r="B118" s="10" t="s">
         <v>365</v>
@@ -5839,7 +5840,7 @@
       <c r="S118" s="10"/>
       <c r="T118" s="10"/>
     </row>
-    <row r="119" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="10"/>
       <c r="B119" s="10" t="s">
         <v>366</v>
@@ -5867,7 +5868,7 @@
       <c r="S119" s="10"/>
       <c r="T119" s="10"/>
     </row>
-    <row r="120" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="10"/>
       <c r="B120" s="10" t="s">
         <v>367</v>
@@ -5895,7 +5896,7 @@
       <c r="S120" s="10"/>
       <c r="T120" s="10"/>
     </row>
-    <row r="121" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="10"/>
       <c r="B121" s="10" t="s">
         <v>368</v>
@@ -5923,7 +5924,7 @@
       <c r="S121" s="10"/>
       <c r="T121" s="10"/>
     </row>
-    <row r="122" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="10"/>
       <c r="B122" s="12" t="s">
         <v>151</v>
@@ -5951,7 +5952,7 @@
       <c r="S122" s="10"/>
       <c r="T122" s="10"/>
     </row>
-    <row r="123" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B123" s="12" t="s">
         <v>152</v>
       </c>
@@ -5971,7 +5972,7 @@
       <c r="S123" s="13"/>
       <c r="T123" s="10"/>
     </row>
-    <row r="124" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B124" s="12" t="s">
         <v>154</v>
       </c>
@@ -5991,7 +5992,7 @@
       <c r="S124" s="13"/>
       <c r="T124" s="10"/>
     </row>
-    <row r="125" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B125" s="10" t="s">
         <v>369</v>
       </c>
@@ -6015,7 +6016,7 @@
       <c r="S125" s="13"/>
       <c r="T125" s="10"/>
     </row>
-    <row r="126" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="10"/>
       <c r="B126" s="10" t="s">
         <v>371</v>
@@ -6043,7 +6044,7 @@
       <c r="S126" s="10"/>
       <c r="T126" s="10"/>
     </row>
-    <row r="127" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="10"/>
       <c r="B127" s="10" t="s">
         <v>372</v>
@@ -6071,7 +6072,7 @@
       <c r="S127" s="10"/>
       <c r="T127" s="10"/>
     </row>
-    <row r="128" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="10"/>
       <c r="B128" s="12" t="s">
         <v>157</v>
@@ -6099,7 +6100,7 @@
       <c r="S128" s="10"/>
       <c r="T128" s="10"/>
     </row>
-    <row r="129" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B129" s="12" t="s">
         <v>158</v>
       </c>
@@ -6116,7 +6117,7 @@
       <c r="S129" s="13"/>
       <c r="T129" s="10"/>
     </row>
-    <row r="130" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B130" s="12" t="s">
         <v>160</v>
       </c>
@@ -6136,7 +6137,7 @@
       <c r="S130" s="13"/>
       <c r="T130" s="10"/>
     </row>
-    <row r="131" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B131" s="12" t="s">
         <v>161</v>
       </c>
@@ -6153,7 +6154,7 @@
       <c r="S131" s="13"/>
       <c r="T131" s="10"/>
     </row>
-    <row r="132" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B132" s="12" t="s">
         <v>162</v>
       </c>
@@ -6170,7 +6171,7 @@
       <c r="S132" s="13"/>
       <c r="T132" s="10"/>
     </row>
-    <row r="133" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B133" s="12" t="s">
         <v>163</v>
       </c>
@@ -6187,7 +6188,7 @@
       <c r="S133" s="13"/>
       <c r="T133" s="10"/>
     </row>
-    <row r="134" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B134" s="12" t="s">
         <v>164</v>
       </c>
@@ -6204,7 +6205,7 @@
       <c r="S134" s="13"/>
       <c r="T134" s="10"/>
     </row>
-    <row r="135" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B135" s="12" t="s">
         <v>165</v>
       </c>
@@ -6221,7 +6222,7 @@
       <c r="S135" s="13"/>
       <c r="T135" s="10"/>
     </row>
-    <row r="136" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B136" s="12" t="s">
         <v>166</v>
       </c>
@@ -6238,7 +6239,7 @@
       <c r="S136" s="13"/>
       <c r="T136" s="10"/>
     </row>
-    <row r="137" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="12" t="s">
         <v>167</v>
       </c>
@@ -6255,7 +6256,7 @@
       <c r="S137" s="13"/>
       <c r="T137" s="10"/>
     </row>
-    <row r="138" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B138" s="12" t="s">
         <v>168</v>
       </c>
@@ -6272,7 +6273,7 @@
       <c r="S138" s="13"/>
       <c r="T138" s="10"/>
     </row>
-    <row r="139" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="12" t="s">
         <v>169</v>
       </c>
@@ -6289,7 +6290,7 @@
       <c r="S139" s="13"/>
       <c r="T139" s="10"/>
     </row>
-    <row r="140" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="12" t="s">
         <v>170</v>
       </c>
@@ -6306,7 +6307,7 @@
       <c r="S140" s="13"/>
       <c r="T140" s="10"/>
     </row>
-    <row r="141" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="12" t="s">
         <v>171</v>
       </c>
@@ -6323,7 +6324,7 @@
       <c r="S141" s="13"/>
       <c r="T141" s="10"/>
     </row>
-    <row r="142" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="10" t="s">
         <v>373</v>
       </c>
@@ -6340,7 +6341,7 @@
       <c r="S142" s="13"/>
       <c r="T142" s="10"/>
     </row>
-    <row r="143" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="10"/>
       <c r="B143" s="10" t="s">
         <v>374</v>
@@ -6368,7 +6369,7 @@
       <c r="S143" s="10"/>
       <c r="T143" s="10"/>
     </row>
-    <row r="144" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="10"/>
       <c r="B144" s="10" t="s">
         <v>375</v>
@@ -6396,7 +6397,7 @@
       <c r="S144" s="10"/>
       <c r="T144" s="10"/>
     </row>
-    <row r="145" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="10"/>
       <c r="B145" s="12" t="s">
         <v>172</v>
@@ -6424,7 +6425,7 @@
       <c r="S145" s="10"/>
       <c r="T145" s="10"/>
     </row>
-    <row r="146" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B146" s="10" t="s">
         <v>376</v>
       </c>
@@ -6441,7 +6442,7 @@
       <c r="S146" s="13"/>
       <c r="T146" s="10"/>
     </row>
-    <row r="147" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="10"/>
       <c r="B147" s="10" t="s">
         <v>377</v>
@@ -6469,7 +6470,7 @@
       <c r="S147" s="10"/>
       <c r="T147" s="10"/>
     </row>
-    <row r="148" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="10"/>
       <c r="B148" s="10" t="s">
         <v>378</v>
@@ -6497,7 +6498,7 @@
       <c r="S148" s="10"/>
       <c r="T148" s="10"/>
     </row>
-    <row r="149" spans="1:20" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" s="12" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A149" s="10"/>
       <c r="B149" s="10" t="s">
         <v>379</v>
@@ -6529,7 +6530,7 @@
       <c r="S149" s="10"/>
       <c r="T149" s="10"/>
     </row>
-    <row r="150" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="10"/>
       <c r="B150" s="10" t="s">
         <v>382</v>
@@ -6555,7 +6556,7 @@
       <c r="S150" s="10"/>
       <c r="T150" s="10"/>
     </row>
-    <row r="151" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="10"/>
       <c r="B151" s="10" t="s">
         <v>383</v>
@@ -6583,7 +6584,7 @@
       <c r="S151" s="10"/>
       <c r="T151" s="10"/>
     </row>
-    <row r="152" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="10"/>
       <c r="B152" s="10" t="s">
         <v>384</v>
@@ -6611,7 +6612,7 @@
       <c r="S152" s="10"/>
       <c r="T152" s="10"/>
     </row>
-    <row r="153" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" s="17" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="16"/>
       <c r="B153" s="16" t="s">
         <v>633</v>
@@ -6647,7 +6648,7 @@
       <c r="S153" s="16"/>
       <c r="T153" s="16"/>
     </row>
-    <row r="154" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="10"/>
       <c r="B154" s="10" t="s">
         <v>385</v>
@@ -6675,7 +6676,7 @@
       <c r="S154" s="10"/>
       <c r="T154" s="10"/>
     </row>
-    <row r="155" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="10"/>
       <c r="B155" s="10" t="s">
         <v>386</v>
@@ -6703,7 +6704,7 @@
       <c r="S155" s="10"/>
       <c r="T155" s="10"/>
     </row>
-    <row r="156" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="10"/>
       <c r="B156" s="10" t="s">
         <v>387</v>
@@ -6731,7 +6732,7 @@
       <c r="S156" s="10"/>
       <c r="T156" s="10"/>
     </row>
-    <row r="157" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="10"/>
       <c r="B157" s="12" t="s">
         <v>173</v>
@@ -6759,7 +6760,7 @@
       <c r="S157" s="10"/>
       <c r="T157" s="10"/>
     </row>
-    <row r="158" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B158" s="10" t="s">
         <v>388</v>
       </c>
@@ -6776,7 +6777,7 @@
       <c r="S158" s="13"/>
       <c r="T158" s="10"/>
     </row>
-    <row r="159" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="10"/>
       <c r="B159" s="10" t="s">
         <v>389</v>
@@ -6810,7 +6811,7 @@
       <c r="S159" s="10"/>
       <c r="T159" s="10"/>
     </row>
-    <row r="160" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="10"/>
       <c r="B160" s="12" t="s">
         <v>174</v>
@@ -6836,7 +6837,7 @@
       <c r="S160" s="10"/>
       <c r="T160" s="10"/>
     </row>
-    <row r="161" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B161" s="10" t="s">
         <v>391</v>
       </c>
@@ -6856,7 +6857,7 @@
       <c r="S161" s="13"/>
       <c r="T161" s="10"/>
     </row>
-    <row r="162" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="10"/>
       <c r="B162" s="10" t="s">
         <v>392</v>
@@ -6884,7 +6885,7 @@
       <c r="S162" s="10"/>
       <c r="T162" s="10"/>
     </row>
-    <row r="163" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="10"/>
       <c r="B163" s="10" t="s">
         <v>394</v>
@@ -6914,7 +6915,7 @@
       <c r="S163" s="10"/>
       <c r="T163" s="10"/>
     </row>
-    <row r="164" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="10"/>
       <c r="B164" s="10" t="s">
         <v>395</v>
@@ -6942,7 +6943,7 @@
       <c r="S164" s="10"/>
       <c r="T164" s="10"/>
     </row>
-    <row r="165" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="10"/>
       <c r="B165" s="10" t="s">
         <v>396</v>
@@ -6970,7 +6971,7 @@
       <c r="S165" s="10"/>
       <c r="T165" s="10"/>
     </row>
-    <row r="166" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="10"/>
       <c r="B166" s="10" t="s">
         <v>397</v>
@@ -6998,7 +6999,7 @@
       <c r="S166" s="10"/>
       <c r="T166" s="10"/>
     </row>
-    <row r="167" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="10"/>
       <c r="B167" s="10" t="s">
         <v>398</v>
@@ -7026,7 +7027,7 @@
       <c r="S167" s="10"/>
       <c r="T167" s="10"/>
     </row>
-    <row r="168" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
       <c r="B168" s="10" t="s">
         <v>399</v>
@@ -7054,7 +7055,7 @@
       <c r="S168" s="10"/>
       <c r="T168" s="10"/>
     </row>
-    <row r="169" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="10"/>
       <c r="B169" s="10" t="s">
         <v>400</v>
@@ -7082,7 +7083,7 @@
       <c r="S169" s="10"/>
       <c r="T169" s="10"/>
     </row>
-    <row r="170" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="10"/>
       <c r="B170" s="10" t="s">
         <v>401</v>
@@ -7110,7 +7111,7 @@
       <c r="S170" s="10"/>
       <c r="T170" s="10"/>
     </row>
-    <row r="171" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="10"/>
       <c r="B171" s="10" t="s">
         <v>402</v>
@@ -7138,7 +7139,7 @@
       <c r="S171" s="10"/>
       <c r="T171" s="10"/>
     </row>
-    <row r="172" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="10"/>
       <c r="B172" s="10" t="s">
         <v>403</v>
@@ -7166,7 +7167,7 @@
       <c r="S172" s="10"/>
       <c r="T172" s="10"/>
     </row>
-    <row r="173" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="10"/>
       <c r="B173" s="10" t="s">
         <v>404</v>
@@ -7194,7 +7195,7 @@
       <c r="S173" s="10"/>
       <c r="T173" s="10"/>
     </row>
-    <row r="174" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="10"/>
       <c r="B174" s="10" t="s">
         <v>405</v>
@@ -7222,7 +7223,7 @@
       <c r="S174" s="10"/>
       <c r="T174" s="10"/>
     </row>
-    <row r="175" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="10"/>
       <c r="B175" s="10" t="s">
         <v>406</v>
@@ -7250,7 +7251,7 @@
       <c r="S175" s="10"/>
       <c r="T175" s="10"/>
     </row>
-    <row r="176" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="10"/>
       <c r="B176" s="12" t="s">
         <v>175</v>
@@ -7280,7 +7281,7 @@
       <c r="S176" s="10"/>
       <c r="T176" s="10"/>
     </row>
-    <row r="177" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="10"/>
       <c r="B177" s="10" t="s">
         <v>407</v>
@@ -7312,7 +7313,7 @@
       <c r="S177" s="10"/>
       <c r="T177" s="10"/>
     </row>
-    <row r="178" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="10"/>
       <c r="B178" s="10" t="s">
         <v>410</v>
@@ -7340,7 +7341,7 @@
       <c r="S178" s="10"/>
       <c r="T178" s="10"/>
     </row>
-    <row r="179" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="10"/>
       <c r="B179" s="10" t="s">
         <v>411</v>
@@ -7368,7 +7369,7 @@
       <c r="S179" s="10"/>
       <c r="T179" s="10"/>
     </row>
-    <row r="180" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="10"/>
       <c r="B180" s="10" t="s">
         <v>412</v>
@@ -7402,7 +7403,7 @@
       <c r="S180" s="10"/>
       <c r="T180" s="10"/>
     </row>
-    <row r="181" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="11"/>
       <c r="B181" s="11" t="s">
         <v>66</v>
@@ -7434,7 +7435,7 @@
       <c r="S181" s="11"/>
       <c r="T181" s="10"/>
     </row>
-    <row r="182" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B182" s="12" t="s">
         <v>176</v>
       </c>
@@ -7451,7 +7452,7 @@
       <c r="S182" s="13"/>
       <c r="T182" s="10"/>
     </row>
-    <row r="183" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B183" s="12" t="s">
         <v>177</v>
       </c>
@@ -7468,7 +7469,7 @@
       <c r="S183" s="13"/>
       <c r="T183" s="10"/>
     </row>
-    <row r="184" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="10"/>
       <c r="B184" s="10" t="s">
         <v>414</v>
@@ -7496,7 +7497,7 @@
       <c r="S184" s="10"/>
       <c r="T184" s="10"/>
     </row>
-    <row r="185" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B185" s="12" t="s">
         <v>178</v>
       </c>
@@ -7513,7 +7514,7 @@
       <c r="S185" s="13"/>
       <c r="T185" s="10"/>
     </row>
-    <row r="186" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="10"/>
       <c r="B186" s="10" t="s">
         <v>415</v>
@@ -7541,7 +7542,7 @@
       <c r="S186" s="10"/>
       <c r="T186" s="10"/>
     </row>
-    <row r="187" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="10"/>
       <c r="B187" s="10" t="s">
         <v>416</v>
@@ -7569,7 +7570,7 @@
       <c r="S187" s="10"/>
       <c r="T187" s="10"/>
     </row>
-    <row r="188" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="10"/>
       <c r="B188" s="10" t="s">
         <v>417</v>
@@ -7597,7 +7598,7 @@
       <c r="S188" s="10"/>
       <c r="T188" s="10"/>
     </row>
-    <row r="189" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="10"/>
       <c r="B189" s="10" t="s">
         <v>418</v>
@@ -7625,7 +7626,7 @@
       <c r="S189" s="10"/>
       <c r="T189" s="10"/>
     </row>
-    <row r="190" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B190" s="12" t="s">
         <v>179</v>
       </c>
@@ -7642,7 +7643,7 @@
       <c r="S190" s="13"/>
       <c r="T190" s="10"/>
     </row>
-    <row r="191" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="10"/>
       <c r="B191" s="10" t="s">
         <v>419</v>
@@ -7670,7 +7671,7 @@
       <c r="S191" s="10"/>
       <c r="T191" s="10"/>
     </row>
-    <row r="192" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="10"/>
       <c r="B192" s="10" t="s">
         <v>420</v>
@@ -7698,7 +7699,7 @@
       <c r="S192" s="10"/>
       <c r="T192" s="10"/>
     </row>
-    <row r="193" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="10"/>
       <c r="B193" s="10" t="s">
         <v>421</v>
@@ -7726,7 +7727,7 @@
       <c r="S193" s="10"/>
       <c r="T193" s="10"/>
     </row>
-    <row r="194" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="10"/>
       <c r="B194" s="10" t="s">
         <v>422</v>
@@ -7754,7 +7755,7 @@
       <c r="S194" s="10"/>
       <c r="T194" s="10"/>
     </row>
-    <row r="195" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="10"/>
       <c r="B195" s="10" t="s">
         <v>423</v>
@@ -7782,7 +7783,7 @@
       <c r="S195" s="10"/>
       <c r="T195" s="10"/>
     </row>
-    <row r="196" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="10"/>
       <c r="B196" s="10" t="s">
         <v>424</v>
@@ -7810,7 +7811,7 @@
       <c r="S196" s="10"/>
       <c r="T196" s="10"/>
     </row>
-    <row r="197" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B197" s="12" t="s">
         <v>180</v>
       </c>
@@ -7827,7 +7828,7 @@
       <c r="S197" s="13"/>
       <c r="T197" s="10"/>
     </row>
-    <row r="198" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="10"/>
       <c r="B198" s="10" t="s">
         <v>425</v>
@@ -7855,7 +7856,7 @@
       <c r="S198" s="10"/>
       <c r="T198" s="10"/>
     </row>
-    <row r="199" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B199" s="12" t="s">
         <v>181</v>
       </c>
@@ -7872,7 +7873,7 @@
       <c r="S199" s="13"/>
       <c r="T199" s="10"/>
     </row>
-    <row r="200" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B200" s="12" t="s">
         <v>182</v>
       </c>
@@ -7889,7 +7890,7 @@
       <c r="S200" s="13"/>
       <c r="T200" s="10"/>
     </row>
-    <row r="201" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B201" s="12" t="s">
         <v>183</v>
       </c>
@@ -7906,7 +7907,7 @@
       <c r="S201" s="13"/>
       <c r="T201" s="10"/>
     </row>
-    <row r="202" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B202" s="12" t="s">
         <v>184</v>
       </c>
@@ -7923,7 +7924,7 @@
       <c r="S202" s="13"/>
       <c r="T202" s="10"/>
     </row>
-    <row r="203" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B203" s="12" t="s">
         <v>185</v>
       </c>
@@ -7940,7 +7941,7 @@
       <c r="S203" s="13"/>
       <c r="T203" s="10"/>
     </row>
-    <row r="204" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B204" s="12" t="s">
         <v>186</v>
       </c>
@@ -7957,7 +7958,7 @@
       <c r="S204" s="13"/>
       <c r="T204" s="10"/>
     </row>
-    <row r="205" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="10"/>
       <c r="B205" s="10" t="s">
         <v>426</v>
@@ -7985,7 +7986,7 @@
       <c r="S205" s="10"/>
       <c r="T205" s="10"/>
     </row>
-    <row r="206" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B206" s="12" t="s">
         <v>187</v>
       </c>
@@ -8002,7 +8003,7 @@
       <c r="S206" s="13"/>
       <c r="T206" s="10"/>
     </row>
-    <row r="207" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="10"/>
       <c r="B207" s="10" t="s">
         <v>427</v>
@@ -8030,7 +8031,7 @@
       <c r="S207" s="10"/>
       <c r="T207" s="10"/>
     </row>
-    <row r="208" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="10"/>
       <c r="B208" s="10" t="s">
         <v>428</v>
@@ -8058,7 +8059,7 @@
       <c r="S208" s="10"/>
       <c r="T208" s="10"/>
     </row>
-    <row r="209" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="10"/>
       <c r="B209" s="10" t="s">
         <v>429</v>
@@ -8086,7 +8087,7 @@
       <c r="S209" s="10"/>
       <c r="T209" s="10"/>
     </row>
-    <row r="210" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="10"/>
       <c r="B210" s="10" t="s">
         <v>430</v>
@@ -8114,7 +8115,7 @@
       <c r="S210" s="10"/>
       <c r="T210" s="10"/>
     </row>
-    <row r="211" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B211" s="12" t="s">
         <v>188</v>
       </c>
@@ -8131,7 +8132,7 @@
       <c r="S211" s="13"/>
       <c r="T211" s="10"/>
     </row>
-    <row r="212" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B212" s="12" t="s">
         <v>189</v>
       </c>
@@ -8151,7 +8152,7 @@
       <c r="S212" s="13"/>
       <c r="T212" s="10"/>
     </row>
-    <row r="213" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="10"/>
       <c r="B213" s="10" t="s">
         <v>431</v>
@@ -8179,7 +8180,7 @@
       <c r="S213" s="10"/>
       <c r="T213" s="10"/>
     </row>
-    <row r="214" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="10"/>
       <c r="B214" s="10" t="s">
         <v>432</v>
@@ -8207,7 +8208,7 @@
       <c r="S214" s="10"/>
       <c r="T214" s="10"/>
     </row>
-    <row r="215" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="10"/>
       <c r="B215" s="10" t="s">
         <v>433</v>
@@ -8235,7 +8236,7 @@
       <c r="S215" s="10"/>
       <c r="T215" s="10"/>
     </row>
-    <row r="216" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="10"/>
       <c r="B216" s="10" t="s">
         <v>434</v>
@@ -8263,7 +8264,7 @@
       <c r="S216" s="10"/>
       <c r="T216" s="10"/>
     </row>
-    <row r="217" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="10"/>
       <c r="B217" s="10" t="s">
         <v>435</v>
@@ -8291,7 +8292,7 @@
       <c r="S217" s="10"/>
       <c r="T217" s="10"/>
     </row>
-    <row r="218" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="10"/>
       <c r="B218" s="10" t="s">
         <v>436</v>
@@ -8319,7 +8320,7 @@
       <c r="S218" s="10"/>
       <c r="T218" s="10"/>
     </row>
-    <row r="219" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B219" s="12" t="s">
         <v>191</v>
       </c>
@@ -8336,7 +8337,7 @@
       <c r="S219" s="13"/>
       <c r="T219" s="10"/>
     </row>
-    <row r="220" spans="1:20" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A220" s="10"/>
       <c r="B220" s="10" t="s">
         <v>437</v>
@@ -8364,7 +8365,7 @@
       <c r="S220" s="10"/>
       <c r="T220" s="10"/>
     </row>
-    <row r="221" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="10"/>
       <c r="B221" s="10" t="s">
         <v>438</v>
@@ -8392,7 +8393,7 @@
       <c r="S221" s="10"/>
       <c r="T221" s="10"/>
     </row>
-    <row r="222" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="10"/>
       <c r="B222" s="10" t="s">
         <v>439</v>
@@ -8422,7 +8423,7 @@
       <c r="S222" s="10"/>
       <c r="T222" s="10"/>
     </row>
-    <row r="223" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A223" s="10"/>
       <c r="B223" s="10" t="s">
         <v>441</v>
@@ -8450,7 +8451,7 @@
       <c r="S223" s="10"/>
       <c r="T223" s="10"/>
     </row>
-    <row r="224" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B224" s="12" t="s">
         <v>192</v>
       </c>
@@ -8467,7 +8468,7 @@
       <c r="S224" s="13"/>
       <c r="T224" s="10"/>
     </row>
-    <row r="225" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="10"/>
       <c r="B225" s="10" t="s">
         <v>442</v>
@@ -8495,7 +8496,7 @@
       <c r="S225" s="10"/>
       <c r="T225" s="10"/>
     </row>
-    <row r="226" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="10"/>
       <c r="B226" s="10" t="s">
         <v>443</v>
@@ -8523,7 +8524,7 @@
       <c r="S226" s="10"/>
       <c r="T226" s="10"/>
     </row>
-    <row r="227" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="10"/>
       <c r="B227" s="10" t="s">
         <v>444</v>
@@ -8551,7 +8552,7 @@
       <c r="S227" s="10"/>
       <c r="T227" s="10"/>
     </row>
-    <row r="228" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="10"/>
       <c r="B228" s="10" t="s">
         <v>445</v>
@@ -8579,7 +8580,7 @@
       <c r="S228" s="10"/>
       <c r="T228" s="10"/>
     </row>
-    <row r="229" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="10"/>
       <c r="B229" s="10" t="s">
         <v>113</v>
@@ -8607,7 +8608,7 @@
       <c r="S229" s="10"/>
       <c r="T229" s="10"/>
     </row>
-    <row r="230" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="10"/>
       <c r="B230" s="10" t="s">
         <v>446</v>
@@ -8635,7 +8636,7 @@
       <c r="S230" s="10"/>
       <c r="T230" s="10"/>
     </row>
-    <row r="231" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="10"/>
       <c r="B231" s="10" t="s">
         <v>447</v>
@@ -8663,7 +8664,7 @@
       <c r="S231" s="10"/>
       <c r="T231" s="10"/>
     </row>
-    <row r="232" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="10"/>
       <c r="B232" s="10" t="s">
         <v>448</v>
@@ -8691,7 +8692,7 @@
       <c r="S232" s="10"/>
       <c r="T232" s="10"/>
     </row>
-    <row r="233" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="10"/>
       <c r="B233" s="10" t="s">
         <v>449</v>
@@ -8719,7 +8720,7 @@
       <c r="S233" s="10"/>
       <c r="T233" s="10"/>
     </row>
-    <row r="234" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A234" s="10"/>
       <c r="B234" s="10" t="s">
         <v>450</v>
@@ -8747,7 +8748,7 @@
       <c r="S234" s="10"/>
       <c r="T234" s="10"/>
     </row>
-    <row r="235" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="10"/>
       <c r="B235" s="10" t="s">
         <v>451</v>
@@ -8775,7 +8776,7 @@
       <c r="S235" s="10"/>
       <c r="T235" s="10"/>
     </row>
-    <row r="236" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B236" s="12" t="s">
         <v>193</v>
       </c>
@@ -8792,7 +8793,7 @@
       <c r="S236" s="13"/>
       <c r="T236" s="10"/>
     </row>
-    <row r="237" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B237" s="12" t="s">
         <v>194</v>
       </c>
@@ -8809,7 +8810,7 @@
       <c r="S237" s="13"/>
       <c r="T237" s="10"/>
     </row>
-    <row r="238" spans="1:20" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:20" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B238" s="12" t="s">
         <v>195</v>
       </c>
@@ -8829,7 +8830,7 @@
       <c r="S238" s="13"/>
       <c r="T238" s="10"/>
     </row>
-    <row r="239" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B239" s="12" t="s">
         <v>197</v>
       </c>
@@ -8846,7 +8847,7 @@
       <c r="S239" s="13"/>
       <c r="T239" s="10"/>
     </row>
-    <row r="240" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A240" s="10"/>
       <c r="B240" s="10" t="s">
         <v>452</v>
@@ -8874,7 +8875,7 @@
       <c r="S240" s="10"/>
       <c r="T240" s="10"/>
     </row>
-    <row r="241" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A241" s="10"/>
       <c r="B241" s="10" t="s">
         <v>453</v>
@@ -8902,7 +8903,7 @@
       <c r="S241" s="10"/>
       <c r="T241" s="10"/>
     </row>
-    <row r="242" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A242" s="10"/>
       <c r="B242" s="10" t="s">
         <v>454</v>
@@ -8930,7 +8931,7 @@
       <c r="S242" s="10"/>
       <c r="T242" s="10"/>
     </row>
-    <row r="243" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A243" s="10"/>
       <c r="B243" s="10" t="s">
         <v>455</v>
@@ -8958,7 +8959,7 @@
       <c r="S243" s="10"/>
       <c r="T243" s="10"/>
     </row>
-    <row r="244" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="10"/>
       <c r="B244" s="10" t="s">
         <v>456</v>
@@ -8986,7 +8987,7 @@
       <c r="S244" s="10"/>
       <c r="T244" s="10"/>
     </row>
-    <row r="245" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A245" s="10"/>
       <c r="B245" s="10" t="s">
         <v>457</v>
@@ -9014,7 +9015,7 @@
       <c r="S245" s="10"/>
       <c r="T245" s="10"/>
     </row>
-    <row r="246" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A246" s="10"/>
       <c r="B246" s="10" t="s">
         <v>458</v>
@@ -9042,7 +9043,7 @@
       <c r="S246" s="10"/>
       <c r="T246" s="10"/>
     </row>
-    <row r="247" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A247" s="10"/>
       <c r="B247" s="10" t="s">
         <v>459</v>
@@ -9070,7 +9071,7 @@
       <c r="S247" s="10"/>
       <c r="T247" s="10"/>
     </row>
-    <row r="248" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" s="10"/>
       <c r="B248" s="10" t="s">
         <v>460</v>
@@ -9098,7 +9099,7 @@
       <c r="S248" s="10"/>
       <c r="T248" s="10"/>
     </row>
-    <row r="249" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" s="10"/>
       <c r="B249" s="10" t="s">
         <v>461</v>
@@ -9128,7 +9129,7 @@
       <c r="S249" s="10"/>
       <c r="T249" s="10"/>
     </row>
-    <row r="250" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A250" s="10"/>
       <c r="B250" s="10" t="s">
         <v>463</v>
@@ -9156,7 +9157,7 @@
       <c r="S250" s="10"/>
       <c r="T250" s="10"/>
     </row>
-    <row r="251" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A251" s="10"/>
       <c r="B251" s="10" t="s">
         <v>464</v>
@@ -9184,7 +9185,7 @@
       <c r="S251" s="10"/>
       <c r="T251" s="10"/>
     </row>
-    <row r="252" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A252" s="10"/>
       <c r="B252" s="10" t="s">
         <v>465</v>
@@ -9212,7 +9213,7 @@
       <c r="S252" s="10"/>
       <c r="T252" s="10"/>
     </row>
-    <row r="253" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A253" s="10"/>
       <c r="B253" s="10" t="s">
         <v>466</v>
@@ -9240,7 +9241,7 @@
       <c r="S253" s="10"/>
       <c r="T253" s="10"/>
     </row>
-    <row r="254" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A254" s="10"/>
       <c r="B254" s="10" t="s">
         <v>467</v>
@@ -9270,7 +9271,7 @@
       <c r="S254" s="10"/>
       <c r="T254" s="10"/>
     </row>
-    <row r="255" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A255" s="10"/>
       <c r="B255" s="10" t="s">
         <v>469</v>
@@ -9298,7 +9299,7 @@
       <c r="S255" s="10"/>
       <c r="T255" s="10"/>
     </row>
-    <row r="256" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A256" s="10"/>
       <c r="B256" s="10" t="s">
         <v>470</v>
@@ -9326,7 +9327,7 @@
       <c r="S256" s="10"/>
       <c r="T256" s="10"/>
     </row>
-    <row r="257" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A257" s="10"/>
       <c r="B257" s="10" t="s">
         <v>471</v>
@@ -9354,7 +9355,7 @@
       <c r="S257" s="10"/>
       <c r="T257" s="10"/>
     </row>
-    <row r="258" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="10"/>
       <c r="B258" s="10" t="s">
         <v>472</v>
@@ -9382,7 +9383,7 @@
       <c r="S258" s="10"/>
       <c r="T258" s="10"/>
     </row>
-    <row r="259" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A259" s="10"/>
       <c r="B259" s="10" t="s">
         <v>473</v>
@@ -9410,7 +9411,7 @@
       <c r="S259" s="10"/>
       <c r="T259" s="10"/>
     </row>
-    <row r="260" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="10"/>
       <c r="B260" s="10" t="s">
         <v>245</v>
@@ -9440,7 +9441,7 @@
       <c r="S260" s="10"/>
       <c r="T260" s="10"/>
     </row>
-    <row r="261" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B261" s="12" t="s">
         <v>126</v>
       </c>
@@ -9460,7 +9461,7 @@
       <c r="S261" s="13"/>
       <c r="T261" s="10"/>
     </row>
-    <row r="262" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B262" s="12" t="s">
         <v>199</v>
       </c>
@@ -9477,7 +9478,7 @@
       <c r="S262" s="13"/>
       <c r="T262" s="10"/>
     </row>
-    <row r="263" spans="1:20" s="30" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:20" s="30" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="B263" s="30" t="s">
         <v>636</v>
       </c>
@@ -9503,7 +9504,7 @@
       <c r="S263" s="29"/>
       <c r="T263" s="31"/>
     </row>
-    <row r="264" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A264" s="10"/>
       <c r="B264" s="10" t="s">
         <v>474</v>
@@ -9531,7 +9532,7 @@
       <c r="S264" s="10"/>
       <c r="T264" s="10"/>
     </row>
-    <row r="265" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A265" s="10"/>
       <c r="B265" s="10" t="s">
         <v>475</v>
@@ -9559,7 +9560,7 @@
       <c r="S265" s="10"/>
       <c r="T265" s="10"/>
     </row>
-    <row r="266" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A266" s="10"/>
       <c r="B266" s="10" t="s">
         <v>476</v>
@@ -9587,7 +9588,7 @@
       <c r="S266" s="10"/>
       <c r="T266" s="10"/>
     </row>
-    <row r="267" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A267" s="10"/>
       <c r="B267" s="10" t="s">
         <v>477</v>
@@ -9615,7 +9616,7 @@
       <c r="S267" s="10"/>
       <c r="T267" s="10"/>
     </row>
-    <row r="268" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A268" s="10"/>
       <c r="B268" s="10" t="s">
         <v>478</v>
@@ -9643,7 +9644,7 @@
       <c r="S268" s="10"/>
       <c r="T268" s="10"/>
     </row>
-    <row r="269" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A269" s="11"/>
       <c r="B269" s="11" t="s">
         <v>65</v>
@@ -9669,7 +9670,7 @@
       <c r="S269" s="11"/>
       <c r="T269" s="10"/>
     </row>
-    <row r="270" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A270" s="10"/>
       <c r="B270" s="10" t="s">
         <v>479</v>
@@ -9697,7 +9698,7 @@
       <c r="S270" s="10"/>
       <c r="T270" s="10"/>
     </row>
-    <row r="271" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A271" s="10"/>
       <c r="B271" s="10" t="s">
         <v>480</v>
@@ -9725,7 +9726,7 @@
       <c r="S271" s="10"/>
       <c r="T271" s="10"/>
     </row>
-    <row r="272" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A272" s="10"/>
       <c r="B272" s="10" t="s">
         <v>481</v>
@@ -9753,7 +9754,7 @@
       <c r="S272" s="10"/>
       <c r="T272" s="10"/>
     </row>
-    <row r="273" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A273" s="10"/>
       <c r="B273" s="10" t="s">
         <v>482</v>
@@ -9781,7 +9782,7 @@
       <c r="S273" s="10"/>
       <c r="T273" s="10"/>
     </row>
-    <row r="274" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A274" s="10"/>
       <c r="B274" s="10" t="s">
         <v>483</v>
@@ -9809,7 +9810,7 @@
       <c r="S274" s="10"/>
       <c r="T274" s="10"/>
     </row>
-    <row r="275" spans="1:20" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:20" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A275" s="10"/>
       <c r="B275" s="13" t="s">
         <v>6</v>
@@ -9845,7 +9846,7 @@
       <c r="S275" s="10"/>
       <c r="T275" s="10"/>
     </row>
-    <row r="276" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A276" s="10"/>
       <c r="B276" s="10" t="s">
         <v>484</v>
@@ -9877,7 +9878,7 @@
       <c r="S276" s="10"/>
       <c r="T276" s="10"/>
     </row>
-    <row r="277" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A277" s="10"/>
       <c r="B277" s="10" t="s">
         <v>487</v>
@@ -9905,7 +9906,7 @@
       <c r="S277" s="10"/>
       <c r="T277" s="10"/>
     </row>
-    <row r="278" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B278" s="12" t="s">
         <v>200</v>
       </c>
@@ -9922,7 +9923,7 @@
       <c r="S278" s="13"/>
       <c r="T278" s="10"/>
     </row>
-    <row r="279" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B279" s="12" t="s">
         <v>201</v>
       </c>
@@ -9939,7 +9940,7 @@
       <c r="S279" s="13"/>
       <c r="T279" s="10"/>
     </row>
-    <row r="280" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B280" s="12" t="s">
         <v>202</v>
       </c>
@@ -9959,7 +9960,7 @@
       <c r="S280" s="13"/>
       <c r="T280" s="10"/>
     </row>
-    <row r="281" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B281" s="12" t="s">
         <v>204</v>
       </c>
@@ -9976,7 +9977,7 @@
       <c r="S281" s="13"/>
       <c r="T281" s="10"/>
     </row>
-    <row r="282" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B282" s="12" t="s">
         <v>205</v>
       </c>
@@ -9993,7 +9994,7 @@
       <c r="S282" s="13"/>
       <c r="T282" s="10"/>
     </row>
-    <row r="283" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B283" s="12" t="s">
         <v>206</v>
       </c>
@@ -10010,7 +10011,7 @@
       <c r="S283" s="13"/>
       <c r="T283" s="10"/>
     </row>
-    <row r="284" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B284" s="12" t="s">
         <v>207</v>
       </c>
@@ -10027,7 +10028,7 @@
       <c r="S284" s="13"/>
       <c r="T284" s="10"/>
     </row>
-    <row r="285" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B285" s="12" t="s">
         <v>208</v>
       </c>
@@ -10044,7 +10045,7 @@
       <c r="S285" s="13"/>
       <c r="T285" s="10"/>
     </row>
-    <row r="286" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B286" s="12" t="s">
         <v>209</v>
       </c>
@@ -10061,7 +10062,7 @@
       <c r="S286" s="13"/>
       <c r="T286" s="10"/>
     </row>
-    <row r="287" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B287" s="12" t="s">
         <v>210</v>
       </c>
@@ -10078,7 +10079,7 @@
       <c r="S287" s="13"/>
       <c r="T287" s="10"/>
     </row>
-    <row r="288" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B288" s="12" t="s">
         <v>211</v>
       </c>
@@ -10095,7 +10096,7 @@
       <c r="S288" s="13"/>
       <c r="T288" s="10"/>
     </row>
-    <row r="289" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B289" s="12" t="s">
         <v>212</v>
       </c>
@@ -10112,7 +10113,7 @@
       <c r="S289" s="13"/>
       <c r="T289" s="10"/>
     </row>
-    <row r="290" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B290" s="12" t="s">
         <v>213</v>
       </c>
@@ -10129,7 +10130,7 @@
       <c r="S290" s="13"/>
       <c r="T290" s="10"/>
     </row>
-    <row r="291" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B291" s="12" t="s">
         <v>214</v>
       </c>
@@ -10146,7 +10147,7 @@
       <c r="S291" s="13"/>
       <c r="T291" s="10"/>
     </row>
-    <row r="292" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B292" s="12" t="s">
         <v>215</v>
       </c>
@@ -10163,7 +10164,7 @@
       <c r="S292" s="13"/>
       <c r="T292" s="10"/>
     </row>
-    <row r="293" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B293" s="12" t="s">
         <v>216</v>
       </c>
@@ -10180,7 +10181,7 @@
       <c r="S293" s="13"/>
       <c r="T293" s="10"/>
     </row>
-    <row r="294" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B294" s="12" t="s">
         <v>217</v>
       </c>
@@ -10197,7 +10198,7 @@
       <c r="S294" s="13"/>
       <c r="T294" s="10"/>
     </row>
-    <row r="295" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A295" s="10"/>
       <c r="B295" s="10" t="s">
         <v>488</v>
@@ -10225,7 +10226,7 @@
       <c r="S295" s="10"/>
       <c r="T295" s="10"/>
     </row>
-    <row r="296" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A296" s="10"/>
       <c r="B296" s="10" t="s">
         <v>489</v>
@@ -10253,7 +10254,7 @@
       <c r="S296" s="10"/>
       <c r="T296" s="10"/>
     </row>
-    <row r="297" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A297" s="10"/>
       <c r="B297" s="10" t="s">
         <v>490</v>
@@ -10281,7 +10282,7 @@
       <c r="S297" s="10"/>
       <c r="T297" s="10"/>
     </row>
-    <row r="298" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B298" s="12" t="s">
         <v>218</v>
       </c>
@@ -10298,7 +10299,7 @@
       <c r="S298" s="13"/>
       <c r="T298" s="10"/>
     </row>
-    <row r="299" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A299" s="10"/>
       <c r="B299" s="10" t="s">
         <v>491</v>
@@ -10326,7 +10327,7 @@
       <c r="S299" s="10"/>
       <c r="T299" s="10"/>
     </row>
-    <row r="300" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A300" s="10"/>
       <c r="B300" s="10" t="s">
         <v>492</v>
@@ -10356,7 +10357,7 @@
       <c r="S300" s="10"/>
       <c r="T300" s="10"/>
     </row>
-    <row r="301" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A301" s="10"/>
       <c r="B301" s="10" t="s">
         <v>494</v>
@@ -10384,7 +10385,7 @@
       <c r="S301" s="10"/>
       <c r="T301" s="10"/>
     </row>
-    <row r="302" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A302" s="10"/>
       <c r="B302" s="10" t="s">
         <v>338</v>
@@ -10412,7 +10413,7 @@
       <c r="S302" s="10"/>
       <c r="T302" s="10"/>
     </row>
-    <row r="303" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B303" s="12" t="s">
         <v>219</v>
       </c>
@@ -10429,7 +10430,7 @@
       <c r="S303" s="13"/>
       <c r="T303" s="10"/>
     </row>
-    <row r="304" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B304" s="12" t="s">
         <v>220</v>
       </c>
@@ -10446,7 +10447,7 @@
       <c r="S304" s="13"/>
       <c r="T304" s="10"/>
     </row>
-    <row r="305" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A305" s="10"/>
       <c r="B305" s="10" t="s">
         <v>495</v>
@@ -10474,7 +10475,7 @@
       <c r="S305" s="10"/>
       <c r="T305" s="10"/>
     </row>
-    <row r="306" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A306" s="10"/>
       <c r="B306" s="10" t="s">
         <v>496</v>
@@ -10502,7 +10503,7 @@
       <c r="S306" s="10"/>
       <c r="T306" s="10"/>
     </row>
-    <row r="307" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A307" s="10"/>
       <c r="B307" s="10" t="s">
         <v>497</v>
@@ -10530,7 +10531,7 @@
       <c r="S307" s="10"/>
       <c r="T307" s="10"/>
     </row>
-    <row r="308" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A308" s="10"/>
       <c r="B308" s="10" t="s">
         <v>498</v>
@@ -10558,7 +10559,7 @@
       <c r="S308" s="10"/>
       <c r="T308" s="10"/>
     </row>
-    <row r="309" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A309" s="10"/>
       <c r="B309" s="10" t="s">
         <v>499</v>
@@ -10586,7 +10587,7 @@
       <c r="S309" s="10"/>
       <c r="T309" s="10"/>
     </row>
-    <row r="310" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A310" s="10"/>
       <c r="B310" s="10" t="s">
         <v>500</v>
@@ -10614,7 +10615,7 @@
       <c r="S310" s="10"/>
       <c r="T310" s="10"/>
     </row>
-    <row r="311" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A311" s="10"/>
       <c r="B311" s="10" t="s">
         <v>501</v>
@@ -10642,7 +10643,7 @@
       <c r="S311" s="10"/>
       <c r="T311" s="10"/>
     </row>
-    <row r="312" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A312" s="10"/>
       <c r="B312" s="10" t="s">
         <v>502</v>
@@ -10670,7 +10671,7 @@
       <c r="S312" s="10"/>
       <c r="T312" s="10"/>
     </row>
-    <row r="313" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A313" s="10"/>
       <c r="B313" s="10" t="s">
         <v>503</v>
@@ -10698,7 +10699,7 @@
       <c r="S313" s="10"/>
       <c r="T313" s="10"/>
     </row>
-    <row r="314" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A314" s="10"/>
       <c r="B314" s="10" t="s">
         <v>504</v>
@@ -10726,7 +10727,7 @@
       <c r="S314" s="10"/>
       <c r="T314" s="10"/>
     </row>
-    <row r="315" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B315" s="12" t="s">
         <v>221</v>
       </c>
@@ -10743,7 +10744,7 @@
       <c r="S315" s="13"/>
       <c r="T315" s="10"/>
     </row>
-    <row r="316" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A316" s="10"/>
       <c r="B316" s="10" t="s">
         <v>505</v>
@@ -10771,7 +10772,7 @@
       <c r="S316" s="10"/>
       <c r="T316" s="10"/>
     </row>
-    <row r="317" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B317" s="12" t="s">
         <v>222</v>
       </c>
@@ -10788,7 +10789,7 @@
       <c r="S317" s="13"/>
       <c r="T317" s="10"/>
     </row>
-    <row r="318" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A318" s="10"/>
       <c r="B318" s="10" t="s">
         <v>506</v>
@@ -10816,7 +10817,7 @@
       <c r="S318" s="10"/>
       <c r="T318" s="10"/>
     </row>
-    <row r="319" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A319" s="10"/>
       <c r="B319" s="10" t="s">
         <v>507</v>
@@ -10844,7 +10845,7 @@
       <c r="S319" s="10"/>
       <c r="T319" s="10"/>
     </row>
-    <row r="320" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A320" s="10"/>
       <c r="B320" s="10" t="s">
         <v>508</v>
@@ -10872,7 +10873,7 @@
       <c r="S320" s="10"/>
       <c r="T320" s="10"/>
     </row>
-    <row r="321" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A321" s="10"/>
       <c r="B321" s="10" t="s">
         <v>509</v>
@@ -10900,7 +10901,7 @@
       <c r="S321" s="10"/>
       <c r="T321" s="10"/>
     </row>
-    <row r="322" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A322" s="10"/>
       <c r="B322" s="10" t="s">
         <v>510</v>
@@ -10928,7 +10929,7 @@
       <c r="S322" s="10"/>
       <c r="T322" s="10"/>
     </row>
-    <row r="323" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A323" s="10"/>
       <c r="B323" s="10" t="s">
         <v>511</v>
@@ -10956,7 +10957,7 @@
       <c r="S323" s="10"/>
       <c r="T323" s="10"/>
     </row>
-    <row r="324" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A324" s="10"/>
       <c r="B324" s="10" t="s">
         <v>512</v>
@@ -10984,7 +10985,7 @@
       <c r="S324" s="10"/>
       <c r="T324" s="10"/>
     </row>
-    <row r="325" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A325" s="10"/>
       <c r="B325" s="10" t="s">
         <v>513</v>
@@ -11012,7 +11013,7 @@
       <c r="S325" s="10"/>
       <c r="T325" s="10"/>
     </row>
-    <row r="326" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A326" s="10"/>
       <c r="B326" s="10" t="s">
         <v>514</v>
@@ -11040,7 +11041,7 @@
       <c r="S326" s="10"/>
       <c r="T326" s="10"/>
     </row>
-    <row r="327" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A327" s="10"/>
       <c r="B327" s="10" t="s">
         <v>515</v>
@@ -11068,7 +11069,7 @@
       <c r="S327" s="10"/>
       <c r="T327" s="10"/>
     </row>
-    <row r="328" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B328" s="12" t="s">
         <v>223</v>
       </c>
@@ -11088,7 +11089,7 @@
       <c r="S328" s="13"/>
       <c r="T328" s="10"/>
     </row>
-    <row r="329" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B329" s="12" t="s">
         <v>224</v>
       </c>
@@ -11105,7 +11106,7 @@
       <c r="S329" s="13"/>
       <c r="T329" s="10"/>
     </row>
-    <row r="330" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A330" s="10"/>
       <c r="B330" s="10" t="s">
         <v>516</v>
@@ -11133,7 +11134,7 @@
       <c r="S330" s="10"/>
       <c r="T330" s="10"/>
     </row>
-    <row r="331" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A331" s="10"/>
       <c r="B331" s="10" t="s">
         <v>517</v>
@@ -11161,7 +11162,7 @@
       <c r="S331" s="10"/>
       <c r="T331" s="10"/>
     </row>
-    <row r="332" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B332" s="12" t="s">
         <v>129</v>
       </c>
@@ -11181,7 +11182,7 @@
       <c r="S332" s="13"/>
       <c r="T332" s="10"/>
     </row>
-    <row r="333" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B333" s="12" t="s">
         <v>226</v>
       </c>
@@ -11201,7 +11202,7 @@
       <c r="S333" s="13"/>
       <c r="T333" s="10"/>
     </row>
-    <row r="334" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B334" s="12" t="s">
         <v>227</v>
       </c>
@@ -11218,7 +11219,7 @@
       <c r="S334" s="13"/>
       <c r="T334" s="10"/>
     </row>
-    <row r="335" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B335" s="12" t="s">
         <v>228</v>
       </c>
@@ -11238,7 +11239,7 @@
       <c r="S335" s="13"/>
       <c r="T335" s="10"/>
     </row>
-    <row r="336" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B336" s="12" t="s">
         <v>229</v>
       </c>
@@ -11255,7 +11256,7 @@
       <c r="S336" s="13"/>
       <c r="T336" s="10"/>
     </row>
-    <row r="337" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B337" s="12" t="s">
         <v>230</v>
       </c>
@@ -11272,7 +11273,7 @@
       <c r="S337" s="13"/>
       <c r="T337" s="10"/>
     </row>
-    <row r="338" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B338" s="12" t="s">
         <v>231</v>
       </c>
@@ -11289,7 +11290,7 @@
       <c r="S338" s="13"/>
       <c r="T338" s="10"/>
     </row>
-    <row r="339" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B339" s="12" t="s">
         <v>131</v>
       </c>
@@ -11306,7 +11307,7 @@
       <c r="S339" s="13"/>
       <c r="T339" s="10"/>
     </row>
-    <row r="340" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B340" s="12" t="s">
         <v>232</v>
       </c>
@@ -11323,7 +11324,7 @@
       <c r="S340" s="13"/>
       <c r="T340" s="10"/>
     </row>
-    <row r="341" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B341" s="12" t="s">
         <v>233</v>
       </c>
@@ -11340,7 +11341,7 @@
       <c r="S341" s="13"/>
       <c r="T341" s="10"/>
     </row>
-    <row r="342" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A342" s="10"/>
       <c r="B342" s="10" t="s">
         <v>518</v>
@@ -11368,7 +11369,7 @@
       <c r="S342" s="10"/>
       <c r="T342" s="10"/>
     </row>
-    <row r="343" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A343" s="10"/>
       <c r="B343" s="10" t="s">
         <v>519</v>
@@ -11396,7 +11397,7 @@
       <c r="S343" s="10"/>
       <c r="T343" s="10"/>
     </row>
-    <row r="344" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A344" s="10"/>
       <c r="B344" s="10" t="s">
         <v>520</v>
@@ -11424,7 +11425,7 @@
       <c r="S344" s="10"/>
       <c r="T344" s="10"/>
     </row>
-    <row r="345" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A345" s="10"/>
       <c r="B345" s="10" t="s">
         <v>521</v>
@@ -11452,7 +11453,7 @@
       <c r="S345" s="10"/>
       <c r="T345" s="10"/>
     </row>
-    <row r="346" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A346" s="10"/>
       <c r="B346" s="10" t="s">
         <v>522</v>
@@ -11480,7 +11481,7 @@
       <c r="S346" s="10"/>
       <c r="T346" s="10"/>
     </row>
-    <row r="347" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A347" s="10"/>
       <c r="B347" s="10" t="s">
         <v>523</v>
@@ -11508,7 +11509,7 @@
       <c r="S347" s="10"/>
       <c r="T347" s="10"/>
     </row>
-    <row r="348" spans="1:20" s="25" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:20" s="25" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A348" s="23"/>
       <c r="B348" s="23" t="s">
         <v>71</v>
@@ -11539,7 +11540,7 @@
       <c r="S348" s="23"/>
       <c r="T348" s="23"/>
     </row>
-    <row r="349" spans="1:20" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:20" s="25" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A349" s="23"/>
       <c r="B349" s="23" t="s">
         <v>524</v>
@@ -11569,7 +11570,7 @@
       <c r="S349" s="23"/>
       <c r="T349" s="23"/>
     </row>
-    <row r="350" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A350" s="10"/>
       <c r="B350" s="10" t="s">
         <v>525</v>
@@ -11597,7 +11598,7 @@
       <c r="S350" s="10"/>
       <c r="T350" s="10"/>
     </row>
-    <row r="351" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A351" s="10"/>
       <c r="B351" s="10" t="s">
         <v>526</v>
@@ -11627,7 +11628,7 @@
       <c r="S351" s="10"/>
       <c r="T351" s="10"/>
     </row>
-    <row r="352" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A352" s="10"/>
       <c r="B352" s="10" t="s">
         <v>528</v>
@@ -11655,7 +11656,7 @@
       <c r="S352" s="10"/>
       <c r="T352" s="10"/>
     </row>
-    <row r="353" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A353" s="10"/>
       <c r="B353" s="10" t="s">
         <v>529</v>
@@ -11683,7 +11684,7 @@
       <c r="S353" s="10"/>
       <c r="T353" s="10"/>
     </row>
-    <row r="354" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A354" s="10"/>
       <c r="B354" s="10" t="s">
         <v>530</v>
@@ -11713,7 +11714,7 @@
       <c r="S354" s="10"/>
       <c r="T354" s="10"/>
     </row>
-    <row r="355" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A355" s="10"/>
       <c r="B355" s="10" t="s">
         <v>532</v>
@@ -11741,7 +11742,7 @@
       <c r="S355" s="10"/>
       <c r="T355" s="10"/>
     </row>
-    <row r="356" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A356" s="10"/>
       <c r="B356" s="10" t="s">
         <v>533</v>
@@ -11771,7 +11772,7 @@
       <c r="S356" s="10"/>
       <c r="T356" s="10"/>
     </row>
-    <row r="357" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A357" s="10"/>
       <c r="B357" s="10" t="s">
         <v>534</v>
@@ -11799,7 +11800,7 @@
       <c r="S357" s="10"/>
       <c r="T357" s="10"/>
     </row>
-    <row r="358" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B358" s="12" t="s">
         <v>234</v>
       </c>
@@ -11816,7 +11817,7 @@
       <c r="S358" s="13"/>
       <c r="T358" s="10"/>
     </row>
-    <row r="359" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B359" s="12" t="s">
         <v>235</v>
       </c>
@@ -11833,7 +11834,7 @@
       <c r="S359" s="13"/>
       <c r="T359" s="10"/>
     </row>
-    <row r="360" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B360" s="12" t="s">
         <v>236</v>
       </c>
@@ -11850,7 +11851,7 @@
       <c r="S360" s="13"/>
       <c r="T360" s="10"/>
     </row>
-    <row r="361" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A361" s="10"/>
       <c r="B361" s="10" t="s">
         <v>535</v>
@@ -11878,7 +11879,7 @@
       <c r="S361" s="10"/>
       <c r="T361" s="10"/>
     </row>
-    <row r="362" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B362" s="12" t="s">
         <v>237</v>
       </c>
@@ -11895,7 +11896,7 @@
       <c r="S362" s="13"/>
       <c r="T362" s="10"/>
     </row>
-    <row r="363" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B363" s="12" t="s">
         <v>238</v>
       </c>
@@ -11912,7 +11913,7 @@
       <c r="S363" s="13"/>
       <c r="T363" s="10"/>
     </row>
-    <row r="364" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B364" s="12" t="s">
         <v>239</v>
       </c>
@@ -11938,7 +11939,7 @@
       <c r="S364" s="13"/>
       <c r="T364" s="10"/>
     </row>
-    <row r="365" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A365" s="10"/>
       <c r="B365" s="10" t="s">
         <v>537</v>
@@ -11970,7 +11971,7 @@
       <c r="S365" s="10"/>
       <c r="T365" s="10"/>
     </row>
-    <row r="366" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B366" s="12" t="s">
         <v>242</v>
       </c>
@@ -11987,7 +11988,7 @@
       <c r="S366" s="13"/>
       <c r="T366" s="10"/>
     </row>
-    <row r="367" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B367" s="12" t="s">
         <v>630</v>
       </c>
@@ -11998,7 +11999,7 @@
       <c r="S367" s="13"/>
       <c r="T367" s="10"/>
     </row>
-    <row r="368" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B368" s="12" t="s">
         <v>243</v>
       </c>
@@ -12024,7 +12025,7 @@
       <c r="S368" s="13"/>
       <c r="T368" s="10"/>
     </row>
-    <row r="369" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B369" s="12" t="s">
         <v>246</v>
       </c>
@@ -12041,7 +12042,7 @@
       <c r="S369" s="13"/>
       <c r="T369" s="10"/>
     </row>
-    <row r="370" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B370" s="12" t="s">
         <v>247</v>
       </c>
@@ -12064,7 +12065,7 @@
       <c r="S370" s="13"/>
       <c r="T370" s="10"/>
     </row>
-    <row r="371" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B371" s="12" t="s">
         <v>250</v>
       </c>
@@ -12081,7 +12082,7 @@
       <c r="S371" s="13"/>
       <c r="T371" s="10"/>
     </row>
-    <row r="372" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A372" s="10"/>
       <c r="B372" s="10" t="s">
         <v>542</v>
@@ -12109,7 +12110,7 @@
       <c r="S372" s="10"/>
       <c r="T372" s="10"/>
     </row>
-    <row r="373" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B373" s="12" t="s">
         <v>251</v>
       </c>
@@ -12126,7 +12127,7 @@
       <c r="S373" s="13"/>
       <c r="T373" s="10"/>
     </row>
-    <row r="374" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A374" s="10"/>
       <c r="B374" s="10" t="s">
         <v>543</v>
@@ -12156,7 +12157,7 @@
       <c r="S374" s="10"/>
       <c r="T374" s="10"/>
     </row>
-    <row r="375" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A375" s="10"/>
       <c r="B375" s="10" t="s">
         <v>545</v>
@@ -12184,7 +12185,7 @@
       <c r="S375" s="10"/>
       <c r="T375" s="10"/>
     </row>
-    <row r="376" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A376" s="10"/>
       <c r="B376" s="10" t="s">
         <v>546</v>
@@ -12212,7 +12213,7 @@
       <c r="S376" s="10"/>
       <c r="T376" s="10"/>
     </row>
-    <row r="377" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A377" s="10"/>
       <c r="B377" s="10" t="s">
         <v>547</v>
@@ -12240,7 +12241,7 @@
       <c r="S377" s="10"/>
       <c r="T377" s="10"/>
     </row>
-    <row r="378" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A378" s="10"/>
       <c r="B378" s="10" t="s">
         <v>548</v>
@@ -12268,7 +12269,7 @@
       <c r="S378" s="10"/>
       <c r="T378" s="10"/>
     </row>
-    <row r="379" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A379" s="10"/>
       <c r="B379" s="10" t="s">
         <v>549</v>
@@ -12296,7 +12297,7 @@
       <c r="S379" s="10"/>
       <c r="T379" s="10"/>
     </row>
-    <row r="380" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A380" s="10"/>
       <c r="B380" s="10" t="s">
         <v>550</v>
@@ -12324,7 +12325,7 @@
       <c r="S380" s="10"/>
       <c r="T380" s="10"/>
     </row>
-    <row r="381" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A381" s="10"/>
       <c r="B381" s="10" t="s">
         <v>551</v>
@@ -12352,7 +12353,7 @@
       <c r="S381" s="10"/>
       <c r="T381" s="10"/>
     </row>
-    <row r="382" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A382" s="10"/>
       <c r="B382" s="10" t="s">
         <v>552</v>
@@ -12380,7 +12381,7 @@
       <c r="S382" s="10"/>
       <c r="T382" s="10"/>
     </row>
-    <row r="383" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A383" s="10"/>
       <c r="B383" s="10" t="s">
         <v>553</v>
@@ -12408,7 +12409,7 @@
       <c r="S383" s="10"/>
       <c r="T383" s="10"/>
     </row>
-    <row r="384" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A384" s="10"/>
       <c r="B384" s="10" t="s">
         <v>554</v>
@@ -12436,7 +12437,7 @@
       <c r="S384" s="10"/>
       <c r="T384" s="10"/>
     </row>
-    <row r="385" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A385" s="10"/>
       <c r="B385" s="10" t="s">
         <v>555</v>
@@ -12464,7 +12465,7 @@
       <c r="S385" s="10"/>
       <c r="T385" s="10"/>
     </row>
-    <row r="386" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A386" s="10"/>
       <c r="B386" s="10" t="s">
         <v>556</v>
@@ -12492,7 +12493,7 @@
       <c r="S386" s="10"/>
       <c r="T386" s="10"/>
     </row>
-    <row r="387" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B387" s="12" t="s">
         <v>136</v>
       </c>
@@ -12512,7 +12513,7 @@
       <c r="S387" s="13"/>
       <c r="T387" s="10"/>
     </row>
-    <row r="388" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B388" s="12" t="s">
         <v>253</v>
       </c>
@@ -12529,7 +12530,7 @@
       <c r="S388" s="13"/>
       <c r="T388" s="10"/>
     </row>
-    <row r="389" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B389" s="12" t="s">
         <v>254</v>
       </c>
@@ -12546,7 +12547,7 @@
       <c r="S389" s="13"/>
       <c r="T389" s="10"/>
     </row>
-    <row r="390" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B390" s="12" t="s">
         <v>255</v>
       </c>
@@ -12563,7 +12564,7 @@
       <c r="S390" s="13"/>
       <c r="T390" s="10"/>
     </row>
-    <row r="391" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B391" s="12" t="s">
         <v>256</v>
       </c>
@@ -12580,7 +12581,7 @@
       <c r="S391" s="13"/>
       <c r="T391" s="10"/>
     </row>
-    <row r="392" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B392" s="12" t="s">
         <v>257</v>
       </c>
@@ -12597,7 +12598,7 @@
       <c r="S392" s="13"/>
       <c r="T392" s="10"/>
     </row>
-    <row r="393" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A393" s="10"/>
       <c r="B393" s="10" t="s">
         <v>557</v>
@@ -12625,7 +12626,7 @@
       <c r="S393" s="10"/>
       <c r="T393" s="10"/>
     </row>
-    <row r="394" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A394" s="10"/>
       <c r="B394" s="10" t="s">
         <v>558</v>
@@ -12653,7 +12654,7 @@
       <c r="S394" s="10"/>
       <c r="T394" s="10"/>
     </row>
-    <row r="395" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A395" s="10"/>
       <c r="B395" s="10" t="s">
         <v>559</v>
@@ -12681,7 +12682,7 @@
       <c r="S395" s="10"/>
       <c r="T395" s="10"/>
     </row>
-    <row r="396" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A396" s="10"/>
       <c r="B396" s="10" t="s">
         <v>560</v>
@@ -12709,7 +12710,7 @@
       <c r="S396" s="10"/>
       <c r="T396" s="10"/>
     </row>
-    <row r="397" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B397" s="12" t="s">
         <v>258</v>
       </c>
@@ -12726,7 +12727,7 @@
       <c r="S397" s="13"/>
       <c r="T397" s="10"/>
     </row>
-    <row r="398" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B398" s="12" t="s">
         <v>259</v>
       </c>
@@ -12743,7 +12744,7 @@
       <c r="S398" s="13"/>
       <c r="T398" s="10"/>
     </row>
-    <row r="399" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A399" s="10"/>
       <c r="B399" s="10" t="s">
         <v>561</v>
@@ -12777,7 +12778,7 @@
       <c r="S399" s="10"/>
       <c r="T399" s="10"/>
     </row>
-    <row r="400" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A400" s="10"/>
       <c r="B400" s="10" t="s">
         <v>563</v>
@@ -12805,7 +12806,7 @@
       <c r="S400" s="10"/>
       <c r="T400" s="10"/>
     </row>
-    <row r="401" spans="2:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B401" s="12" t="s">
         <v>260</v>
       </c>
@@ -12822,7 +12823,7 @@
       <c r="S401" s="13"/>
       <c r="T401" s="10"/>
     </row>
-    <row r="402" spans="2:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B402" s="12" t="s">
         <v>261</v>
       </c>
@@ -12839,13 +12840,13 @@
       <c r="S402" s="13"/>
       <c r="T402" s="10"/>
     </row>
-    <row r="403" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:20" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B403" s="13"/>
       <c r="Q403" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="404" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B404" s="13"/>
       <c r="G404" s="11"/>
       <c r="H404" s="11"/>
@@ -12861,25 +12862,25 @@
       <c r="P404" s="11"/>
       <c r="Q404" s="11"/>
     </row>
-    <row r="405" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:20" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B405" s="13"/>
       <c r="Q405" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="406" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:20" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B406" s="13"/>
       <c r="Q406" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="407" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:20" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B407" s="13"/>
       <c r="Q407" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="408" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B408" s="13"/>
       <c r="E408" s="11"/>
       <c r="F408" s="11"/>
@@ -12895,13 +12896,13 @@
       <c r="P408" s="11"/>
       <c r="Q408" s="11"/>
     </row>
-    <row r="409" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:20" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B409" s="13"/>
       <c r="Q409" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="410" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B410" s="13"/>
       <c r="C410" s="11"/>
       <c r="D410" s="21"/>
@@ -12919,7 +12920,7 @@
       <c r="P410" s="11"/>
       <c r="Q410" s="11"/>
     </row>
-    <row r="411" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B411" s="13"/>
       <c r="C411" s="11"/>
       <c r="D411" s="21"/>
@@ -12937,44 +12938,44 @@
       <c r="P411" s="11"/>
       <c r="Q411" s="11"/>
     </row>
-    <row r="412" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B412" s="13"/>
       <c r="R412" s="11"/>
     </row>
-    <row r="413" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B413" s="13"/>
     </row>
-    <row r="414" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B414" s="13"/>
     </row>
-    <row r="415" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B415" s="13"/>
     </row>
-    <row r="416" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B416" s="13"/>
     </row>
-    <row r="417" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B417" s="13"/>
     </row>
-    <row r="418" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B418" s="13"/>
     </row>
-    <row r="419" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B419" s="13"/>
     </row>
-    <row r="420" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B420" s="13"/>
     </row>
-    <row r="421" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A421" s="13"/>
       <c r="B421" s="13"/>
       <c r="S421" s="11"/>
     </row>
-    <row r="422" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B422" s="13"/>
       <c r="R422" s="11"/>
     </row>
-    <row r="423" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B423" s="13"/>
       <c r="C423" s="11"/>
       <c r="D423" s="21"/>
@@ -12992,7 +12993,7 @@
       <c r="P423" s="11"/>
       <c r="Q423" s="11"/>
     </row>
-    <row r="424" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B424" s="13"/>
       <c r="C424" s="11"/>
       <c r="D424" s="21"/>
@@ -13011,7 +13012,7 @@
       <c r="Q424" s="11"/>
       <c r="R424" s="11"/>
     </row>
-    <row r="425" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A425" s="11"/>
       <c r="B425" s="13"/>
       <c r="C425" s="11"/>
@@ -13032,7 +13033,7 @@
       <c r="R425" s="11"/>
       <c r="S425" s="11"/>
     </row>
-    <row r="426" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B426" s="13"/>
       <c r="C426" s="11"/>
       <c r="D426" s="21"/>
@@ -13051,7 +13052,7 @@
       <c r="Q426" s="11"/>
       <c r="R426" s="11"/>
     </row>
-    <row r="427" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B427" s="13"/>
     </row>
   </sheetData>
@@ -13064,23 +13065,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="93" style="4" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="45.1640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>83</v>
       </c>
@@ -13094,7 +13095,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -13105,7 +13106,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -13116,7 +13117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -13130,7 +13131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -13141,7 +13142,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>60</v>
       </c>
@@ -13155,7 +13156,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>82</v>
       </c>
@@ -13166,7 +13167,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>74</v>
       </c>
@@ -13177,7 +13178,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
@@ -13188,7 +13189,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>67</v>
       </c>
@@ -13199,7 +13200,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>75</v>
       </c>
@@ -13210,7 +13211,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
@@ -13221,7 +13222,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
@@ -13232,7 +13233,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>79</v>
       </c>
@@ -13243,7 +13244,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>114</v>
       </c>
@@ -13254,7 +13255,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>115</v>
       </c>
@@ -13265,7 +13266,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>116</v>
       </c>
@@ -13276,7 +13277,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>117</v>
       </c>
@@ -13287,7 +13288,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>580</v>
       </c>
@@ -13305,29 +13306,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="36.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="36.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -13365,7 +13366,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -13379,7 +13380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
@@ -13393,7 +13394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -13410,7 +13411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
@@ -13421,7 +13422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
@@ -13435,7 +13436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
@@ -13452,7 +13453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -13466,7 +13467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
@@ -13483,7 +13484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="42" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
@@ -13503,14 +13504,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13518,19 +13519,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="43.28515625" customWidth="1"/>
+    <col min="11" max="11" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>32</v>
       </c>
@@ -13565,7 +13566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13576,7 +13577,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13593,7 +13594,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13610,7 +13611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13627,7 +13628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13644,7 +13645,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13661,7 +13662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13678,7 +13679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13695,7 +13696,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -13712,7 +13713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -13729,7 +13730,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -13755,7 +13756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13781,7 +13782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13807,7 +13808,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13833,7 +13834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13859,7 +13860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13885,7 +13886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13911,7 +13912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13937,7 +13938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13963,7 +13964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -13989,7 +13990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -14015,7 +14016,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -14041,7 +14042,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -14067,7 +14068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -14093,7 +14094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -14119,7 +14120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -14145,7 +14146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -14171,7 +14172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -14197,7 +14198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>

</xml_diff>